<commit_message>
show data for crashes per 1000 registered vehicles
</commit_message>
<xml_diff>
--- a/misc/unfaelle-kanton.xlsx
+++ b/misc/unfaelle-kanton.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hinri\Source\Repos\ivis_traffic\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B9550-5509-4B8C-81B3-ABF858BBD3F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444A3ADA-4EE0-487D-BDBC-38ED48F92D50}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10040" activeTab="2" xr2:uid="{C1D9424B-A159-4C57-A0A7-78A5565826A5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10040" activeTab="3" xr2:uid="{C1D9424B-A159-4C57-A0A7-78A5565826A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Originaldaten" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
     <sheet name="Export" sheetId="1" r:id="rId3"/>
+    <sheet name="Normalise" sheetId="5" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Originaldaten!$A$1:$AB$235</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -447,6 +451,2026 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Raw data"/>
+      <sheetName val="Pivot"/>
+      <sheetName val="Export"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="B2">
+            <v>236043</v>
+          </cell>
+          <cell r="C2">
+            <v>239081</v>
+          </cell>
+          <cell r="D2">
+            <v>244652</v>
+          </cell>
+          <cell r="E2">
+            <v>249590</v>
+          </cell>
+          <cell r="F2">
+            <v>254808</v>
+          </cell>
+          <cell r="G2">
+            <v>259639</v>
+          </cell>
+          <cell r="H2">
+            <v>265854</v>
+          </cell>
+          <cell r="I2">
+            <v>273313</v>
+          </cell>
+          <cell r="J2">
+            <v>280261</v>
+          </cell>
+          <cell r="K2">
+            <v>287399</v>
+          </cell>
+          <cell r="L2">
+            <v>294212</v>
+          </cell>
+          <cell r="M2">
+            <v>300916</v>
+          </cell>
+          <cell r="N2">
+            <v>306571</v>
+          </cell>
+          <cell r="O2">
+            <v>311370</v>
+          </cell>
+          <cell r="P2">
+            <v>316298</v>
+          </cell>
+          <cell r="Q2">
+            <v>321731</v>
+          </cell>
+          <cell r="R2">
+            <v>327074</v>
+          </cell>
+          <cell r="S2">
+            <v>329151</v>
+          </cell>
+          <cell r="T2">
+            <v>339424</v>
+          </cell>
+          <cell r="U2">
+            <v>348117</v>
+          </cell>
+          <cell r="V2">
+            <v>357099</v>
+          </cell>
+          <cell r="W2">
+            <v>364771</v>
+          </cell>
+          <cell r="X2">
+            <v>371223</v>
+          </cell>
+          <cell r="Y2">
+            <v>378078</v>
+          </cell>
+          <cell r="Z2">
+            <v>385642</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>22418</v>
+          </cell>
+          <cell r="C3">
+            <v>22860</v>
+          </cell>
+          <cell r="D3">
+            <v>23306</v>
+          </cell>
+          <cell r="E3">
+            <v>23409</v>
+          </cell>
+          <cell r="F3">
+            <v>21340</v>
+          </cell>
+          <cell r="G3">
+            <v>23990</v>
+          </cell>
+          <cell r="H3">
+            <v>24081</v>
+          </cell>
+          <cell r="I3">
+            <v>24949</v>
+          </cell>
+          <cell r="J3">
+            <v>25345</v>
+          </cell>
+          <cell r="K3">
+            <v>25663</v>
+          </cell>
+          <cell r="L3">
+            <v>26040</v>
+          </cell>
+          <cell r="M3">
+            <v>26402</v>
+          </cell>
+          <cell r="N3">
+            <v>26904</v>
+          </cell>
+          <cell r="O3">
+            <v>27053</v>
+          </cell>
+          <cell r="P3">
+            <v>26490</v>
+          </cell>
+          <cell r="Q3">
+            <v>26933</v>
+          </cell>
+          <cell r="R3">
+            <v>27631</v>
+          </cell>
+          <cell r="S3">
+            <v>28733</v>
+          </cell>
+          <cell r="T3">
+            <v>27580</v>
+          </cell>
+          <cell r="U3">
+            <v>28376</v>
+          </cell>
+          <cell r="V3">
+            <v>29144</v>
+          </cell>
+          <cell r="W3">
+            <v>29696</v>
+          </cell>
+          <cell r="X3">
+            <v>30312</v>
+          </cell>
+          <cell r="Y3">
+            <v>30874</v>
+          </cell>
+          <cell r="Z3">
+            <v>31345</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>5565</v>
+          </cell>
+          <cell r="C4">
+            <v>5711</v>
+          </cell>
+          <cell r="D4">
+            <v>5728</v>
+          </cell>
+          <cell r="E4">
+            <v>5803</v>
+          </cell>
+          <cell r="F4">
+            <v>5394</v>
+          </cell>
+          <cell r="G4">
+            <v>6081</v>
+          </cell>
+          <cell r="H4">
+            <v>6136</v>
+          </cell>
+          <cell r="I4">
+            <v>6313</v>
+          </cell>
+          <cell r="J4">
+            <v>6461</v>
+          </cell>
+          <cell r="K4">
+            <v>6678</v>
+          </cell>
+          <cell r="L4">
+            <v>6837</v>
+          </cell>
+          <cell r="M4">
+            <v>6975</v>
+          </cell>
+          <cell r="N4">
+            <v>7153</v>
+          </cell>
+          <cell r="O4">
+            <v>7349</v>
+          </cell>
+          <cell r="P4">
+            <v>7421</v>
+          </cell>
+          <cell r="Q4">
+            <v>7635</v>
+          </cell>
+          <cell r="R4">
+            <v>7731</v>
+          </cell>
+          <cell r="S4">
+            <v>8243</v>
+          </cell>
+          <cell r="T4">
+            <v>8286</v>
+          </cell>
+          <cell r="U4">
+            <v>8518</v>
+          </cell>
+          <cell r="V4">
+            <v>8654</v>
+          </cell>
+          <cell r="W4">
+            <v>8808</v>
+          </cell>
+          <cell r="X4">
+            <v>8951</v>
+          </cell>
+          <cell r="Y4">
+            <v>9246</v>
+          </cell>
+          <cell r="Z4">
+            <v>9456</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>100133</v>
+          </cell>
+          <cell r="C5">
+            <v>101209</v>
+          </cell>
+          <cell r="D5">
+            <v>110188</v>
+          </cell>
+          <cell r="E5">
+            <v>112172</v>
+          </cell>
+          <cell r="F5">
+            <v>113542</v>
+          </cell>
+          <cell r="G5">
+            <v>115819</v>
+          </cell>
+          <cell r="H5">
+            <v>118395</v>
+          </cell>
+          <cell r="I5">
+            <v>121536</v>
+          </cell>
+          <cell r="J5">
+            <v>124367</v>
+          </cell>
+          <cell r="K5">
+            <v>127043</v>
+          </cell>
+          <cell r="L5">
+            <v>129485</v>
+          </cell>
+          <cell r="M5">
+            <v>131523</v>
+          </cell>
+          <cell r="N5">
+            <v>132804</v>
+          </cell>
+          <cell r="O5">
+            <v>133190</v>
+          </cell>
+          <cell r="P5">
+            <v>134693</v>
+          </cell>
+          <cell r="Q5">
+            <v>134394</v>
+          </cell>
+          <cell r="R5">
+            <v>136417</v>
+          </cell>
+          <cell r="S5">
+            <v>143092</v>
+          </cell>
+          <cell r="T5">
+            <v>138195</v>
+          </cell>
+          <cell r="U5">
+            <v>139882</v>
+          </cell>
+          <cell r="V5">
+            <v>141538</v>
+          </cell>
+          <cell r="W5">
+            <v>142222</v>
+          </cell>
+          <cell r="X5">
+            <v>143596</v>
+          </cell>
+          <cell r="Y5">
+            <v>145003</v>
+          </cell>
+          <cell r="Z5">
+            <v>146631</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>64510</v>
+          </cell>
+          <cell r="C6">
+            <v>64079</v>
+          </cell>
+          <cell r="D6">
+            <v>63967</v>
+          </cell>
+          <cell r="E6">
+            <v>63876</v>
+          </cell>
+          <cell r="F6">
+            <v>63735</v>
+          </cell>
+          <cell r="G6">
+            <v>63241</v>
+          </cell>
+          <cell r="H6">
+            <v>63417</v>
+          </cell>
+          <cell r="I6">
+            <v>63982</v>
+          </cell>
+          <cell r="J6">
+            <v>64044</v>
+          </cell>
+          <cell r="K6">
+            <v>64675</v>
+          </cell>
+          <cell r="L6">
+            <v>64724</v>
+          </cell>
+          <cell r="M6">
+            <v>65455</v>
+          </cell>
+          <cell r="N6">
+            <v>65212</v>
+          </cell>
+          <cell r="O6">
+            <v>66279</v>
+          </cell>
+          <cell r="P6">
+            <v>64812</v>
+          </cell>
+          <cell r="Q6">
+            <v>64700</v>
+          </cell>
+          <cell r="R6">
+            <v>65319</v>
+          </cell>
+          <cell r="S6">
+            <v>64339</v>
+          </cell>
+          <cell r="T6">
+            <v>66077</v>
+          </cell>
+          <cell r="U6">
+            <v>66523</v>
+          </cell>
+          <cell r="V6">
+            <v>67356</v>
+          </cell>
+          <cell r="W6">
+            <v>66805</v>
+          </cell>
+          <cell r="X6">
+            <v>67028</v>
+          </cell>
+          <cell r="Y6">
+            <v>65741</v>
+          </cell>
+          <cell r="Z6">
+            <v>65956</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>393552</v>
+          </cell>
+          <cell r="C7">
+            <v>393976</v>
+          </cell>
+          <cell r="D7">
+            <v>391440</v>
+          </cell>
+          <cell r="E7">
+            <v>399943</v>
+          </cell>
+          <cell r="F7">
+            <v>396217</v>
+          </cell>
+          <cell r="G7">
+            <v>403029</v>
+          </cell>
+          <cell r="H7">
+            <v>410672</v>
+          </cell>
+          <cell r="I7">
+            <v>420001</v>
+          </cell>
+          <cell r="J7">
+            <v>429355</v>
+          </cell>
+          <cell r="K7">
+            <v>439226</v>
+          </cell>
+          <cell r="L7">
+            <v>448988</v>
+          </cell>
+          <cell r="M7">
+            <v>455819</v>
+          </cell>
+          <cell r="N7">
+            <v>461589</v>
+          </cell>
+          <cell r="O7">
+            <v>465327</v>
+          </cell>
+          <cell r="P7">
+            <v>478545</v>
+          </cell>
+          <cell r="Q7">
+            <v>481257</v>
+          </cell>
+          <cell r="R7">
+            <v>487023</v>
+          </cell>
+          <cell r="S7">
+            <v>471407</v>
+          </cell>
+          <cell r="T7">
+            <v>480990</v>
+          </cell>
+          <cell r="U7">
+            <v>488368</v>
+          </cell>
+          <cell r="V7">
+            <v>496854</v>
+          </cell>
+          <cell r="W7">
+            <v>504791</v>
+          </cell>
+          <cell r="X7">
+            <v>512043</v>
+          </cell>
+          <cell r="Y7">
+            <v>519826</v>
+          </cell>
+          <cell r="Z7">
+            <v>527314</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>100572</v>
+          </cell>
+          <cell r="C8">
+            <v>102373</v>
+          </cell>
+          <cell r="D8">
+            <v>105124</v>
+          </cell>
+          <cell r="E8">
+            <v>108064</v>
+          </cell>
+          <cell r="F8">
+            <v>110726</v>
+          </cell>
+          <cell r="G8">
+            <v>113251</v>
+          </cell>
+          <cell r="H8">
+            <v>115705</v>
+          </cell>
+          <cell r="I8">
+            <v>119163</v>
+          </cell>
+          <cell r="J8">
+            <v>122182</v>
+          </cell>
+          <cell r="K8">
+            <v>125567</v>
+          </cell>
+          <cell r="L8">
+            <v>128866</v>
+          </cell>
+          <cell r="M8">
+            <v>131608</v>
+          </cell>
+          <cell r="N8">
+            <v>134381</v>
+          </cell>
+          <cell r="O8">
+            <v>136866</v>
+          </cell>
+          <cell r="P8">
+            <v>140577</v>
+          </cell>
+          <cell r="Q8">
+            <v>142995</v>
+          </cell>
+          <cell r="R8">
+            <v>147724</v>
+          </cell>
+          <cell r="S8">
+            <v>155560</v>
+          </cell>
+          <cell r="T8">
+            <v>154180</v>
+          </cell>
+          <cell r="U8">
+            <v>158902</v>
+          </cell>
+          <cell r="V8">
+            <v>164212</v>
+          </cell>
+          <cell r="W8">
+            <v>168351</v>
+          </cell>
+          <cell r="X8">
+            <v>172240</v>
+          </cell>
+          <cell r="Y8">
+            <v>176522</v>
+          </cell>
+          <cell r="Z8">
+            <v>180259</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>192717</v>
+          </cell>
+          <cell r="C9">
+            <v>191917</v>
+          </cell>
+          <cell r="D9">
+            <v>194254</v>
+          </cell>
+          <cell r="E9">
+            <v>197234</v>
+          </cell>
+          <cell r="F9">
+            <v>199956</v>
+          </cell>
+          <cell r="G9">
+            <v>202029</v>
+          </cell>
+          <cell r="H9">
+            <v>204237</v>
+          </cell>
+          <cell r="I9">
+            <v>207496</v>
+          </cell>
+          <cell r="J9">
+            <v>212902</v>
+          </cell>
+          <cell r="K9">
+            <v>217772</v>
+          </cell>
+          <cell r="L9">
+            <v>220854</v>
+          </cell>
+          <cell r="M9">
+            <v>222358</v>
+          </cell>
+          <cell r="N9">
+            <v>223642</v>
+          </cell>
+          <cell r="O9">
+            <v>224694</v>
+          </cell>
+          <cell r="P9">
+            <v>222710</v>
+          </cell>
+          <cell r="Q9">
+            <v>221251</v>
+          </cell>
+          <cell r="R9">
+            <v>217702</v>
+          </cell>
+          <cell r="S9">
+            <v>215009</v>
+          </cell>
+          <cell r="T9">
+            <v>216504</v>
+          </cell>
+          <cell r="U9">
+            <v>218270</v>
+          </cell>
+          <cell r="V9">
+            <v>219766</v>
+          </cell>
+          <cell r="W9">
+            <v>219275</v>
+          </cell>
+          <cell r="X9">
+            <v>219636</v>
+          </cell>
+          <cell r="Y9">
+            <v>221143</v>
+          </cell>
+          <cell r="Z9">
+            <v>221757</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>16075</v>
+          </cell>
+          <cell r="C10">
+            <v>16142</v>
+          </cell>
+          <cell r="D10">
+            <v>16426</v>
+          </cell>
+          <cell r="E10">
+            <v>16746</v>
+          </cell>
+          <cell r="F10">
+            <v>15389</v>
+          </cell>
+          <cell r="G10">
+            <v>17038</v>
+          </cell>
+          <cell r="H10">
+            <v>17108</v>
+          </cell>
+          <cell r="I10">
+            <v>17462</v>
+          </cell>
+          <cell r="J10">
+            <v>17686</v>
+          </cell>
+          <cell r="K10">
+            <v>18022</v>
+          </cell>
+          <cell r="L10">
+            <v>18447</v>
+          </cell>
+          <cell r="M10">
+            <v>18802</v>
+          </cell>
+          <cell r="N10">
+            <v>19137</v>
+          </cell>
+          <cell r="O10">
+            <v>19308</v>
+          </cell>
+          <cell r="P10">
+            <v>18558</v>
+          </cell>
+          <cell r="Q10">
+            <v>18903</v>
+          </cell>
+          <cell r="R10">
+            <v>18965</v>
+          </cell>
+          <cell r="S10">
+            <v>20047</v>
+          </cell>
+          <cell r="T10">
+            <v>20651</v>
+          </cell>
+          <cell r="U10">
+            <v>21242</v>
+          </cell>
+          <cell r="V10">
+            <v>21822</v>
+          </cell>
+          <cell r="W10">
+            <v>22225</v>
+          </cell>
+          <cell r="X10">
+            <v>22572</v>
+          </cell>
+          <cell r="Y10">
+            <v>23013</v>
+          </cell>
+          <cell r="Z10">
+            <v>23231</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>76593</v>
+          </cell>
+          <cell r="C11">
+            <v>77869</v>
+          </cell>
+          <cell r="D11">
+            <v>79681</v>
+          </cell>
+          <cell r="E11">
+            <v>81410</v>
+          </cell>
+          <cell r="F11">
+            <v>82564</v>
+          </cell>
+          <cell r="G11">
+            <v>82607</v>
+          </cell>
+          <cell r="H11">
+            <v>83438</v>
+          </cell>
+          <cell r="I11">
+            <v>84901</v>
+          </cell>
+          <cell r="J11">
+            <v>85829</v>
+          </cell>
+          <cell r="K11">
+            <v>86926</v>
+          </cell>
+          <cell r="L11">
+            <v>88213</v>
+          </cell>
+          <cell r="M11">
+            <v>89505</v>
+          </cell>
+          <cell r="N11">
+            <v>90779</v>
+          </cell>
+          <cell r="O11">
+            <v>92251</v>
+          </cell>
+          <cell r="P11">
+            <v>94140</v>
+          </cell>
+          <cell r="Q11">
+            <v>95744</v>
+          </cell>
+          <cell r="R11">
+            <v>97940</v>
+          </cell>
+          <cell r="S11">
+            <v>101032</v>
+          </cell>
+          <cell r="T11">
+            <v>100122</v>
+          </cell>
+          <cell r="U11">
+            <v>102308</v>
+          </cell>
+          <cell r="V11">
+            <v>104538</v>
+          </cell>
+          <cell r="W11">
+            <v>106006</v>
+          </cell>
+          <cell r="X11">
+            <v>107662</v>
+          </cell>
+          <cell r="Y11">
+            <v>109262</v>
+          </cell>
+          <cell r="Z11">
+            <v>110726</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>30106</v>
+          </cell>
+          <cell r="C12">
+            <v>30242</v>
+          </cell>
+          <cell r="D12">
+            <v>30987</v>
+          </cell>
+          <cell r="E12">
+            <v>31432</v>
+          </cell>
+          <cell r="F12">
+            <v>32086</v>
+          </cell>
+          <cell r="G12">
+            <v>32920</v>
+          </cell>
+          <cell r="H12">
+            <v>33523</v>
+          </cell>
+          <cell r="I12">
+            <v>34253</v>
+          </cell>
+          <cell r="J12">
+            <v>34575</v>
+          </cell>
+          <cell r="K12">
+            <v>35110</v>
+          </cell>
+          <cell r="L12">
+            <v>35446</v>
+          </cell>
+          <cell r="M12">
+            <v>36015</v>
+          </cell>
+          <cell r="N12">
+            <v>36472</v>
+          </cell>
+          <cell r="O12">
+            <v>36913</v>
+          </cell>
+          <cell r="P12">
+            <v>36981</v>
+          </cell>
+          <cell r="Q12">
+            <v>37548</v>
+          </cell>
+          <cell r="R12">
+            <v>37888</v>
+          </cell>
+          <cell r="S12">
+            <v>37801</v>
+          </cell>
+          <cell r="T12">
+            <v>38600</v>
+          </cell>
+          <cell r="U12">
+            <v>39412</v>
+          </cell>
+          <cell r="V12">
+            <v>40077</v>
+          </cell>
+          <cell r="W12">
+            <v>40942</v>
+          </cell>
+          <cell r="X12">
+            <v>41438</v>
+          </cell>
+          <cell r="Y12">
+            <v>41989</v>
+          </cell>
+          <cell r="Z12">
+            <v>42575</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>133163</v>
+          </cell>
+          <cell r="C13">
+            <v>135175</v>
+          </cell>
+          <cell r="D13">
+            <v>137775</v>
+          </cell>
+          <cell r="E13">
+            <v>140035</v>
+          </cell>
+          <cell r="F13">
+            <v>142408</v>
+          </cell>
+          <cell r="G13">
+            <v>144233</v>
+          </cell>
+          <cell r="H13">
+            <v>146888</v>
+          </cell>
+          <cell r="I13">
+            <v>150544</v>
+          </cell>
+          <cell r="J13">
+            <v>154246</v>
+          </cell>
+          <cell r="K13">
+            <v>158329</v>
+          </cell>
+          <cell r="L13">
+            <v>161707</v>
+          </cell>
+          <cell r="M13">
+            <v>163576</v>
+          </cell>
+          <cell r="N13">
+            <v>166508</v>
+          </cell>
+          <cell r="O13">
+            <v>168848</v>
+          </cell>
+          <cell r="P13">
+            <v>171365</v>
+          </cell>
+          <cell r="Q13">
+            <v>175335</v>
+          </cell>
+          <cell r="R13">
+            <v>178789</v>
+          </cell>
+          <cell r="S13">
+            <v>180089</v>
+          </cell>
+          <cell r="T13">
+            <v>185867</v>
+          </cell>
+          <cell r="U13">
+            <v>190978</v>
+          </cell>
+          <cell r="V13">
+            <v>196171</v>
+          </cell>
+          <cell r="W13">
+            <v>200121</v>
+          </cell>
+          <cell r="X13">
+            <v>204286</v>
+          </cell>
+          <cell r="Y13">
+            <v>209062</v>
+          </cell>
+          <cell r="Z13">
+            <v>213061</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>76439</v>
+          </cell>
+          <cell r="C14">
+            <v>76463</v>
+          </cell>
+          <cell r="D14">
+            <v>77394</v>
+          </cell>
+          <cell r="E14">
+            <v>78795</v>
+          </cell>
+          <cell r="F14">
+            <v>80708</v>
+          </cell>
+          <cell r="G14">
+            <v>81325</v>
+          </cell>
+          <cell r="H14">
+            <v>81974</v>
+          </cell>
+          <cell r="I14">
+            <v>83039</v>
+          </cell>
+          <cell r="J14">
+            <v>84563</v>
+          </cell>
+          <cell r="K14">
+            <v>85733</v>
+          </cell>
+          <cell r="L14">
+            <v>86549</v>
+          </cell>
+          <cell r="M14">
+            <v>87004</v>
+          </cell>
+          <cell r="N14">
+            <v>87796</v>
+          </cell>
+          <cell r="O14">
+            <v>87734</v>
+          </cell>
+          <cell r="P14">
+            <v>86894</v>
+          </cell>
+          <cell r="Q14">
+            <v>87511</v>
+          </cell>
+          <cell r="R14">
+            <v>88117</v>
+          </cell>
+          <cell r="S14">
+            <v>88526</v>
+          </cell>
+          <cell r="T14">
+            <v>89980</v>
+          </cell>
+          <cell r="U14">
+            <v>91713</v>
+          </cell>
+          <cell r="V14">
+            <v>93517</v>
+          </cell>
+          <cell r="W14">
+            <v>94890</v>
+          </cell>
+          <cell r="X14">
+            <v>95191</v>
+          </cell>
+          <cell r="Y14">
+            <v>96255</v>
+          </cell>
+          <cell r="Z14">
+            <v>96938</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>16209</v>
+          </cell>
+          <cell r="C15">
+            <v>16485</v>
+          </cell>
+          <cell r="D15">
+            <v>16760</v>
+          </cell>
+          <cell r="E15">
+            <v>17149</v>
+          </cell>
+          <cell r="F15">
+            <v>16348</v>
+          </cell>
+          <cell r="G15">
+            <v>18495</v>
+          </cell>
+          <cell r="H15">
+            <v>18574</v>
+          </cell>
+          <cell r="I15">
+            <v>19237</v>
+          </cell>
+          <cell r="J15">
+            <v>19943</v>
+          </cell>
+          <cell r="K15">
+            <v>20632</v>
+          </cell>
+          <cell r="L15">
+            <v>21151</v>
+          </cell>
+          <cell r="M15">
+            <v>21344</v>
+          </cell>
+          <cell r="N15">
+            <v>21917</v>
+          </cell>
+          <cell r="O15">
+            <v>21988</v>
+          </cell>
+          <cell r="P15">
+            <v>21813</v>
+          </cell>
+          <cell r="Q15">
+            <v>22280</v>
+          </cell>
+          <cell r="R15">
+            <v>22415</v>
+          </cell>
+          <cell r="S15">
+            <v>23389</v>
+          </cell>
+          <cell r="T15">
+            <v>23874</v>
+          </cell>
+          <cell r="U15">
+            <v>24369</v>
+          </cell>
+          <cell r="V15">
+            <v>24837</v>
+          </cell>
+          <cell r="W15">
+            <v>25341</v>
+          </cell>
+          <cell r="X15">
+            <v>25705</v>
+          </cell>
+          <cell r="Y15">
+            <v>26049</v>
+          </cell>
+          <cell r="Z15">
+            <v>26430</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>12891</v>
+          </cell>
+          <cell r="C16">
+            <v>13134</v>
+          </cell>
+          <cell r="D16">
+            <v>13532</v>
+          </cell>
+          <cell r="E16">
+            <v>13945</v>
+          </cell>
+          <cell r="F16">
+            <v>12959</v>
+          </cell>
+          <cell r="G16">
+            <v>14628</v>
+          </cell>
+          <cell r="H16">
+            <v>14839</v>
+          </cell>
+          <cell r="I16">
+            <v>15543</v>
+          </cell>
+          <cell r="J16">
+            <v>15826</v>
+          </cell>
+          <cell r="K16">
+            <v>16233</v>
+          </cell>
+          <cell r="L16">
+            <v>16651</v>
+          </cell>
+          <cell r="M16">
+            <v>16987</v>
+          </cell>
+          <cell r="N16">
+            <v>17189</v>
+          </cell>
+          <cell r="O16">
+            <v>17220</v>
+          </cell>
+          <cell r="P16">
+            <v>17297</v>
+          </cell>
+          <cell r="Q16">
+            <v>17725</v>
+          </cell>
+          <cell r="R16">
+            <v>17932</v>
+          </cell>
+          <cell r="S16">
+            <v>18782</v>
+          </cell>
+          <cell r="T16">
+            <v>19542</v>
+          </cell>
+          <cell r="U16">
+            <v>20110</v>
+          </cell>
+          <cell r="V16">
+            <v>20701</v>
+          </cell>
+          <cell r="W16">
+            <v>21091</v>
+          </cell>
+          <cell r="X16">
+            <v>21454</v>
+          </cell>
+          <cell r="Y16">
+            <v>21771</v>
+          </cell>
+          <cell r="Z16">
+            <v>22042</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>31994</v>
+          </cell>
+          <cell r="C17">
+            <v>32103</v>
+          </cell>
+          <cell r="D17">
+            <v>32574</v>
+          </cell>
+          <cell r="E17">
+            <v>32829</v>
+          </cell>
+          <cell r="F17">
+            <v>33856</v>
+          </cell>
+          <cell r="G17">
+            <v>33776</v>
+          </cell>
+          <cell r="H17">
+            <v>34460</v>
+          </cell>
+          <cell r="I17">
+            <v>35146</v>
+          </cell>
+          <cell r="J17">
+            <v>35888</v>
+          </cell>
+          <cell r="K17">
+            <v>36660</v>
+          </cell>
+          <cell r="L17">
+            <v>37515</v>
+          </cell>
+          <cell r="M17">
+            <v>38242</v>
+          </cell>
+          <cell r="N17">
+            <v>38729</v>
+          </cell>
+          <cell r="O17">
+            <v>39159</v>
+          </cell>
+          <cell r="P17">
+            <v>38219</v>
+          </cell>
+          <cell r="Q17">
+            <v>38957</v>
+          </cell>
+          <cell r="R17">
+            <v>39711</v>
+          </cell>
+          <cell r="S17">
+            <v>39078</v>
+          </cell>
+          <cell r="T17">
+            <v>40311</v>
+          </cell>
+          <cell r="U17">
+            <v>41437</v>
+          </cell>
+          <cell r="V17">
+            <v>42334</v>
+          </cell>
+          <cell r="W17">
+            <v>43024</v>
+          </cell>
+          <cell r="X17">
+            <v>43785</v>
+          </cell>
+          <cell r="Y17">
+            <v>44296</v>
+          </cell>
+          <cell r="Z17">
+            <v>44970</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>53710</v>
+          </cell>
+          <cell r="C18">
+            <v>55469</v>
+          </cell>
+          <cell r="D18">
+            <v>57290</v>
+          </cell>
+          <cell r="E18">
+            <v>59021</v>
+          </cell>
+          <cell r="F18">
+            <v>60457</v>
+          </cell>
+          <cell r="G18">
+            <v>61876</v>
+          </cell>
+          <cell r="H18">
+            <v>63566</v>
+          </cell>
+          <cell r="I18">
+            <v>65954</v>
+          </cell>
+          <cell r="J18">
+            <v>67984</v>
+          </cell>
+          <cell r="K18">
+            <v>70678</v>
+          </cell>
+          <cell r="L18">
+            <v>72983</v>
+          </cell>
+          <cell r="M18">
+            <v>74448</v>
+          </cell>
+          <cell r="N18">
+            <v>76468</v>
+          </cell>
+          <cell r="O18">
+            <v>77768</v>
+          </cell>
+          <cell r="P18">
+            <v>76528</v>
+          </cell>
+          <cell r="Q18">
+            <v>79809</v>
+          </cell>
+          <cell r="R18">
+            <v>81805</v>
+          </cell>
+          <cell r="S18">
+            <v>83108</v>
+          </cell>
+          <cell r="T18">
+            <v>86245</v>
+          </cell>
+          <cell r="U18">
+            <v>88593</v>
+          </cell>
+          <cell r="V18">
+            <v>91168</v>
+          </cell>
+          <cell r="W18">
+            <v>92766</v>
+          </cell>
+          <cell r="X18">
+            <v>94458</v>
+          </cell>
+          <cell r="Y18">
+            <v>96378</v>
+          </cell>
+          <cell r="Z18">
+            <v>98477</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>106566</v>
+          </cell>
+          <cell r="C19">
+            <v>105010</v>
+          </cell>
+          <cell r="D19">
+            <v>106659</v>
+          </cell>
+          <cell r="E19">
+            <v>109549</v>
+          </cell>
+          <cell r="F19">
+            <v>111296</v>
+          </cell>
+          <cell r="G19">
+            <v>112671</v>
+          </cell>
+          <cell r="H19">
+            <v>115465</v>
+          </cell>
+          <cell r="I19">
+            <v>118417</v>
+          </cell>
+          <cell r="J19">
+            <v>121243</v>
+          </cell>
+          <cell r="K19">
+            <v>124110</v>
+          </cell>
+          <cell r="L19">
+            <v>126974</v>
+          </cell>
+          <cell r="M19">
+            <v>129378</v>
+          </cell>
+          <cell r="N19">
+            <v>131042</v>
+          </cell>
+          <cell r="O19">
+            <v>133473</v>
+          </cell>
+          <cell r="P19">
+            <v>133213</v>
+          </cell>
+          <cell r="Q19">
+            <v>134991</v>
+          </cell>
+          <cell r="R19">
+            <v>135941</v>
+          </cell>
+          <cell r="S19">
+            <v>136240</v>
+          </cell>
+          <cell r="T19">
+            <v>139864</v>
+          </cell>
+          <cell r="U19">
+            <v>142534</v>
+          </cell>
+          <cell r="V19">
+            <v>145972</v>
+          </cell>
+          <cell r="W19">
+            <v>148322</v>
+          </cell>
+          <cell r="X19">
+            <v>150356</v>
+          </cell>
+          <cell r="Y19">
+            <v>152385</v>
+          </cell>
+          <cell r="Z19">
+            <v>155081</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>172881</v>
+          </cell>
+          <cell r="C20">
+            <v>174807</v>
+          </cell>
+          <cell r="D20">
+            <v>178914</v>
+          </cell>
+          <cell r="E20">
+            <v>183589</v>
+          </cell>
+          <cell r="F20">
+            <v>187277</v>
+          </cell>
+          <cell r="G20">
+            <v>189418</v>
+          </cell>
+          <cell r="H20">
+            <v>193455</v>
+          </cell>
+          <cell r="I20">
+            <v>198436</v>
+          </cell>
+          <cell r="J20">
+            <v>203260</v>
+          </cell>
+          <cell r="K20">
+            <v>208618</v>
+          </cell>
+          <cell r="L20">
+            <v>214271</v>
+          </cell>
+          <cell r="M20">
+            <v>218103</v>
+          </cell>
+          <cell r="N20">
+            <v>222317</v>
+          </cell>
+          <cell r="O20">
+            <v>224047</v>
+          </cell>
+          <cell r="P20">
+            <v>228737</v>
+          </cell>
+          <cell r="Q20">
+            <v>231267</v>
+          </cell>
+          <cell r="R20">
+            <v>232637</v>
+          </cell>
+          <cell r="S20">
+            <v>238473</v>
+          </cell>
+          <cell r="T20">
+            <v>246075</v>
+          </cell>
+          <cell r="U20">
+            <v>252838</v>
+          </cell>
+          <cell r="V20">
+            <v>259581</v>
+          </cell>
+          <cell r="W20">
+            <v>264860</v>
+          </cell>
+          <cell r="X20">
+            <v>268737</v>
+          </cell>
+          <cell r="Y20">
+            <v>272067</v>
+          </cell>
+          <cell r="Z20">
+            <v>275969</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>95589</v>
+          </cell>
+          <cell r="C21">
+            <v>97338</v>
+          </cell>
+          <cell r="D21">
+            <v>100901</v>
+          </cell>
+          <cell r="E21">
+            <v>103324</v>
+          </cell>
+          <cell r="F21">
+            <v>105241</v>
+          </cell>
+          <cell r="G21">
+            <v>106601</v>
+          </cell>
+          <cell r="H21">
+            <v>108156</v>
+          </cell>
+          <cell r="I21">
+            <v>111402</v>
+          </cell>
+          <cell r="J21">
+            <v>114401</v>
+          </cell>
+          <cell r="K21">
+            <v>117629</v>
+          </cell>
+          <cell r="L21">
+            <v>120567</v>
+          </cell>
+          <cell r="M21">
+            <v>123245</v>
+          </cell>
+          <cell r="N21">
+            <v>125209</v>
+          </cell>
+          <cell r="O21">
+            <v>126377</v>
+          </cell>
+          <cell r="P21">
+            <v>129898</v>
+          </cell>
+          <cell r="Q21">
+            <v>131559</v>
+          </cell>
+          <cell r="R21">
+            <v>137042</v>
+          </cell>
+          <cell r="S21">
+            <v>145313</v>
+          </cell>
+          <cell r="T21">
+            <v>142616</v>
+          </cell>
+          <cell r="U21">
+            <v>147056</v>
+          </cell>
+          <cell r="V21">
+            <v>151919</v>
+          </cell>
+          <cell r="W21">
+            <v>155407</v>
+          </cell>
+          <cell r="X21">
+            <v>159528</v>
+          </cell>
+          <cell r="Y21">
+            <v>163678</v>
+          </cell>
+          <cell r="Z21">
+            <v>167035</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>157260</v>
+          </cell>
+          <cell r="C22">
+            <v>160109</v>
+          </cell>
+          <cell r="D22">
+            <v>163845</v>
+          </cell>
+          <cell r="E22">
+            <v>167561</v>
+          </cell>
+          <cell r="F22">
+            <v>170164</v>
+          </cell>
+          <cell r="G22">
+            <v>172584</v>
+          </cell>
+          <cell r="H22">
+            <v>175749</v>
+          </cell>
+          <cell r="I22">
+            <v>179394</v>
+          </cell>
+          <cell r="J22">
+            <v>182624</v>
+          </cell>
+          <cell r="K22">
+            <v>185979</v>
+          </cell>
+          <cell r="L22">
+            <v>188109</v>
+          </cell>
+          <cell r="M22">
+            <v>188428</v>
+          </cell>
+          <cell r="N22">
+            <v>191130</v>
+          </cell>
+          <cell r="O22">
+            <v>193374</v>
+          </cell>
+          <cell r="P22">
+            <v>195473</v>
+          </cell>
+          <cell r="Q22">
+            <v>198713</v>
+          </cell>
+          <cell r="R22">
+            <v>200122</v>
+          </cell>
+          <cell r="S22">
+            <v>202068</v>
+          </cell>
+          <cell r="T22">
+            <v>204462</v>
+          </cell>
+          <cell r="U22">
+            <v>208141</v>
+          </cell>
+          <cell r="V22">
+            <v>211697</v>
+          </cell>
+          <cell r="W22">
+            <v>215106</v>
+          </cell>
+          <cell r="X22">
+            <v>218839</v>
+          </cell>
+          <cell r="Y22">
+            <v>222243</v>
+          </cell>
+          <cell r="Z22">
+            <v>224565</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>13740</v>
+          </cell>
+          <cell r="C23">
+            <v>13936</v>
+          </cell>
+          <cell r="D23">
+            <v>14281</v>
+          </cell>
+          <cell r="E23">
+            <v>14480</v>
+          </cell>
+          <cell r="F23">
+            <v>13393</v>
+          </cell>
+          <cell r="G23">
+            <v>15012</v>
+          </cell>
+          <cell r="H23">
+            <v>15091</v>
+          </cell>
+          <cell r="I23">
+            <v>15848</v>
+          </cell>
+          <cell r="J23">
+            <v>15750</v>
+          </cell>
+          <cell r="K23">
+            <v>15999</v>
+          </cell>
+          <cell r="L23">
+            <v>16307</v>
+          </cell>
+          <cell r="M23">
+            <v>16585</v>
+          </cell>
+          <cell r="N23">
+            <v>16686</v>
+          </cell>
+          <cell r="O23">
+            <v>16685</v>
+          </cell>
+          <cell r="P23">
+            <v>16138</v>
+          </cell>
+          <cell r="Q23">
+            <v>16332</v>
+          </cell>
+          <cell r="R23">
+            <v>16331</v>
+          </cell>
+          <cell r="S23">
+            <v>17240</v>
+          </cell>
+          <cell r="T23">
+            <v>17699</v>
+          </cell>
+          <cell r="U23">
+            <v>18019</v>
+          </cell>
+          <cell r="V23">
+            <v>18444</v>
+          </cell>
+          <cell r="W23">
+            <v>18756</v>
+          </cell>
+          <cell r="X23">
+            <v>19018</v>
+          </cell>
+          <cell r="Y23">
+            <v>19346</v>
+          </cell>
+          <cell r="Z23">
+            <v>19563</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>127080</v>
+          </cell>
+          <cell r="C24">
+            <v>128358</v>
+          </cell>
+          <cell r="D24">
+            <v>130793</v>
+          </cell>
+          <cell r="E24">
+            <v>132981</v>
+          </cell>
+          <cell r="F24">
+            <v>136337</v>
+          </cell>
+          <cell r="G24">
+            <v>138774</v>
+          </cell>
+          <cell r="H24">
+            <v>142282</v>
+          </cell>
+          <cell r="I24">
+            <v>145984</v>
+          </cell>
+          <cell r="J24">
+            <v>148643</v>
+          </cell>
+          <cell r="K24">
+            <v>152579</v>
+          </cell>
+          <cell r="L24">
+            <v>156589</v>
+          </cell>
+          <cell r="M24">
+            <v>160561</v>
+          </cell>
+          <cell r="N24">
+            <v>163359</v>
+          </cell>
+          <cell r="O24">
+            <v>166673</v>
+          </cell>
+          <cell r="P24">
+            <v>170647</v>
+          </cell>
+          <cell r="Q24">
+            <v>174007</v>
+          </cell>
+          <cell r="R24">
+            <v>175605</v>
+          </cell>
+          <cell r="S24">
+            <v>181230</v>
+          </cell>
+          <cell r="T24">
+            <v>185530</v>
+          </cell>
+          <cell r="U24">
+            <v>191508</v>
+          </cell>
+          <cell r="V24">
+            <v>197712</v>
+          </cell>
+          <cell r="W24">
+            <v>201380</v>
+          </cell>
+          <cell r="X24">
+            <v>205075</v>
+          </cell>
+          <cell r="Y24">
+            <v>209439</v>
+          </cell>
+          <cell r="Z24">
+            <v>213611</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>285141</v>
+          </cell>
+          <cell r="C25">
+            <v>285286</v>
+          </cell>
+          <cell r="D25">
+            <v>290504</v>
+          </cell>
+          <cell r="E25">
+            <v>296014</v>
+          </cell>
+          <cell r="F25">
+            <v>301230</v>
+          </cell>
+          <cell r="G25">
+            <v>306791</v>
+          </cell>
+          <cell r="H25">
+            <v>313138</v>
+          </cell>
+          <cell r="I25">
+            <v>323067</v>
+          </cell>
+          <cell r="J25">
+            <v>330654</v>
+          </cell>
+          <cell r="K25">
+            <v>337893</v>
+          </cell>
+          <cell r="L25">
+            <v>342505</v>
+          </cell>
+          <cell r="M25">
+            <v>347813</v>
+          </cell>
+          <cell r="N25">
+            <v>353119</v>
+          </cell>
+          <cell r="O25">
+            <v>353999</v>
+          </cell>
+          <cell r="P25">
+            <v>351776</v>
+          </cell>
+          <cell r="Q25">
+            <v>355741</v>
+          </cell>
+          <cell r="R25">
+            <v>361110</v>
+          </cell>
+          <cell r="S25">
+            <v>357553</v>
+          </cell>
+          <cell r="T25">
+            <v>366762</v>
+          </cell>
+          <cell r="U25">
+            <v>375399</v>
+          </cell>
+          <cell r="V25">
+            <v>384687</v>
+          </cell>
+          <cell r="W25">
+            <v>391740</v>
+          </cell>
+          <cell r="X25">
+            <v>397551</v>
+          </cell>
+          <cell r="Y25">
+            <v>403749</v>
+          </cell>
+          <cell r="Z25">
+            <v>410283</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>42292</v>
+          </cell>
+          <cell r="C26">
+            <v>43348</v>
+          </cell>
+          <cell r="D26">
+            <v>44457</v>
+          </cell>
+          <cell r="E26">
+            <v>45618</v>
+          </cell>
+          <cell r="F26">
+            <v>47176</v>
+          </cell>
+          <cell r="G26">
+            <v>48607</v>
+          </cell>
+          <cell r="H26">
+            <v>50553</v>
+          </cell>
+          <cell r="I26">
+            <v>52603</v>
+          </cell>
+          <cell r="J26">
+            <v>54606</v>
+          </cell>
+          <cell r="K26">
+            <v>56581</v>
+          </cell>
+          <cell r="L26">
+            <v>58176</v>
+          </cell>
+          <cell r="M26">
+            <v>59425</v>
+          </cell>
+          <cell r="N26">
+            <v>60511</v>
+          </cell>
+          <cell r="O26">
+            <v>62206</v>
+          </cell>
+          <cell r="P26">
+            <v>61928</v>
+          </cell>
+          <cell r="Q26">
+            <v>63392</v>
+          </cell>
+          <cell r="R26">
+            <v>64963</v>
+          </cell>
+          <cell r="S26">
+            <v>65159</v>
+          </cell>
+          <cell r="T26">
+            <v>66963</v>
+          </cell>
+          <cell r="U26">
+            <v>68959</v>
+          </cell>
+          <cell r="V26">
+            <v>71061</v>
+          </cell>
+          <cell r="W26">
+            <v>72770</v>
+          </cell>
+          <cell r="X26">
+            <v>74798</v>
+          </cell>
+          <cell r="Y26">
+            <v>76957</v>
+          </cell>
+          <cell r="Z26">
+            <v>79137</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>521888</v>
+          </cell>
+          <cell r="C27">
+            <v>521023</v>
+          </cell>
+          <cell r="D27">
+            <v>527619</v>
+          </cell>
+          <cell r="E27">
+            <v>538764</v>
+          </cell>
+          <cell r="F27">
+            <v>547536</v>
+          </cell>
+          <cell r="G27">
+            <v>553113</v>
+          </cell>
+          <cell r="H27">
+            <v>564472</v>
+          </cell>
+          <cell r="I27">
+            <v>577241</v>
+          </cell>
+          <cell r="J27">
+            <v>590758</v>
+          </cell>
+          <cell r="K27">
+            <v>606207</v>
+          </cell>
+          <cell r="L27">
+            <v>617047</v>
+          </cell>
+          <cell r="M27">
+            <v>622878</v>
+          </cell>
+          <cell r="N27">
+            <v>634529</v>
+          </cell>
+          <cell r="O27">
+            <v>651102</v>
+          </cell>
+          <cell r="P27">
+            <v>658731</v>
+          </cell>
+          <cell r="Q27">
+            <v>674948</v>
+          </cell>
+          <cell r="R27">
+            <v>665751</v>
+          </cell>
+          <cell r="S27">
+            <v>658814</v>
+          </cell>
+          <cell r="T27">
+            <v>669381</v>
+          </cell>
+          <cell r="U27">
+            <v>681387</v>
+          </cell>
+          <cell r="V27">
+            <v>693864</v>
+          </cell>
+          <cell r="W27">
+            <v>701419</v>
+          </cell>
+          <cell r="X27">
+            <v>709008</v>
+          </cell>
+          <cell r="Y27">
+            <v>723697</v>
+          </cell>
+          <cell r="Z27">
+            <v>731975</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7716,7 +9740,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5BFA8EC-EA80-4CB0-AB16-D16AC6739F16}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B5BFA8EC-EA80-4CB0-AB16-D16AC6739F16}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:Z30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="28">
     <pivotField axis="axisRow" showAll="0">
@@ -30974,13 +32998,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1304E66-5B2C-4161-8A08-9C56FD39812C}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
@@ -33791,6 +35815,2883 @@
       <c r="Z27">
         <f>Pivot!Z29</f>
         <v>3410</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C6432-729C-48F7-9D3A-D9BF03A7BDE3}">
+  <dimension ref="A1:Z27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" t="str">
+        <f>Export!A1</f>
+        <v>Kanton</v>
+      </c>
+      <c r="B1">
+        <f>Export!B1</f>
+        <v>1992</v>
+      </c>
+      <c r="C1">
+        <f>Export!C1</f>
+        <v>1993</v>
+      </c>
+      <c r="D1">
+        <f>Export!D1</f>
+        <v>1994</v>
+      </c>
+      <c r="E1">
+        <f>Export!E1</f>
+        <v>1995</v>
+      </c>
+      <c r="F1">
+        <f>Export!F1</f>
+        <v>1996</v>
+      </c>
+      <c r="G1">
+        <f>Export!G1</f>
+        <v>1997</v>
+      </c>
+      <c r="H1">
+        <f>Export!H1</f>
+        <v>1998</v>
+      </c>
+      <c r="I1">
+        <f>Export!I1</f>
+        <v>1999</v>
+      </c>
+      <c r="J1">
+        <f>Export!J1</f>
+        <v>2000</v>
+      </c>
+      <c r="K1">
+        <f>Export!K1</f>
+        <v>2001</v>
+      </c>
+      <c r="L1">
+        <f>Export!L1</f>
+        <v>2002</v>
+      </c>
+      <c r="M1">
+        <f>Export!M1</f>
+        <v>2003</v>
+      </c>
+      <c r="N1">
+        <f>Export!N1</f>
+        <v>2004</v>
+      </c>
+      <c r="O1">
+        <f>Export!O1</f>
+        <v>2005</v>
+      </c>
+      <c r="P1">
+        <f>Export!P1</f>
+        <v>2006</v>
+      </c>
+      <c r="Q1">
+        <f>Export!Q1</f>
+        <v>2007</v>
+      </c>
+      <c r="R1">
+        <f>Export!R1</f>
+        <v>2008</v>
+      </c>
+      <c r="S1">
+        <f>Export!S1</f>
+        <v>2009</v>
+      </c>
+      <c r="T1">
+        <f>Export!T1</f>
+        <v>2010</v>
+      </c>
+      <c r="U1">
+        <f>Export!U1</f>
+        <v>2011</v>
+      </c>
+      <c r="V1">
+        <f>Export!V1</f>
+        <v>2012</v>
+      </c>
+      <c r="W1">
+        <f>Export!W1</f>
+        <v>2013</v>
+      </c>
+      <c r="X1">
+        <f>Export!X1</f>
+        <v>2014</v>
+      </c>
+      <c r="Y1">
+        <f>Export!Y1</f>
+        <v>2015</v>
+      </c>
+      <c r="Z1">
+        <f>Export!Z1</f>
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>Export!A2</f>
+        <v>AG</v>
+      </c>
+      <c r="B2">
+        <f>(1000*Export!B2)/[1]Export!B2</f>
+        <v>6.553890604677961</v>
+      </c>
+      <c r="C2">
+        <f>(1000*Export!C2)/[1]Export!C2</f>
+        <v>6.4036874532062358</v>
+      </c>
+      <c r="D2">
+        <f>(1000*Export!D2)/[1]Export!D2</f>
+        <v>6.911858476529928</v>
+      </c>
+      <c r="E2">
+        <f>(1000*Export!E2)/[1]Export!E2</f>
+        <v>6.3143555430906684</v>
+      </c>
+      <c r="F2">
+        <f>(1000*Export!F2)/[1]Export!F2</f>
+        <v>6.059464381024144</v>
+      </c>
+      <c r="G2">
+        <f>(1000*Export!G2)/[1]Export!G2</f>
+        <v>5.7156282376684553</v>
+      </c>
+      <c r="H2">
+        <f>(1000*Export!H2)/[1]Export!H2</f>
+        <v>5.3826536369586311</v>
+      </c>
+      <c r="I2">
+        <f>(1000*Export!I2)/[1]Export!I2</f>
+        <v>6.3004686934028022</v>
+      </c>
+      <c r="J2">
+        <f>(1000*Export!J2)/[1]Export!J2</f>
+        <v>6.0158209668844398</v>
+      </c>
+      <c r="K2">
+        <f>(1000*Export!K2)/[1]Export!K2</f>
+        <v>5.9429573519740844</v>
+      </c>
+      <c r="L2">
+        <f>(1000*Export!L2)/[1]Export!L2</f>
+        <v>5.8087365573124146</v>
+      </c>
+      <c r="M2">
+        <f>(1000*Export!M2)/[1]Export!M2</f>
+        <v>5.2140796767204138</v>
+      </c>
+      <c r="N2">
+        <f>(1000*Export!N2)/[1]Export!N2</f>
+        <v>4.9058782468009046</v>
+      </c>
+      <c r="O2">
+        <f>(1000*Export!O2)/[1]Export!O2</f>
+        <v>4.9523075440793907</v>
+      </c>
+      <c r="P2">
+        <f>(1000*Export!P2)/[1]Export!P2</f>
+        <v>4.7139090351503965</v>
+      </c>
+      <c r="Q2">
+        <f>(1000*Export!Q2)/[1]Export!Q2</f>
+        <v>4.6591717925844884</v>
+      </c>
+      <c r="R2">
+        <f>(1000*Export!R2)/[1]Export!R2</f>
+        <v>4.3048362144346539</v>
+      </c>
+      <c r="S2">
+        <f>(1000*Export!S2)/[1]Export!S2</f>
+        <v>4.4478066297838987</v>
+      </c>
+      <c r="T2">
+        <f>(1000*Export!T2)/[1]Export!T2</f>
+        <v>3.962595455831055</v>
+      </c>
+      <c r="U2">
+        <f>(1000*Export!U2)/[1]Export!U2</f>
+        <v>3.9009873117371456</v>
+      </c>
+      <c r="V2">
+        <f>(1000*Export!V2)/[1]Export!V2</f>
+        <v>3.5004298527859219</v>
+      </c>
+      <c r="W2">
+        <f>(1000*Export!W2)/[1]Export!W2</f>
+        <v>3.2650621897025807</v>
+      </c>
+      <c r="X2">
+        <f>(1000*Export!X2)/[1]Export!X2</f>
+        <v>3.2729653065677504</v>
+      </c>
+      <c r="Y2">
+        <f>(1000*Export!Y2)/[1]Export!Y2</f>
+        <v>3.2083326720941181</v>
+      </c>
+      <c r="Z2">
+        <f>(1000*Export!Z2)/[1]Export!Z2</f>
+        <v>2.797931760544754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>Export!A3</f>
+        <v>AR</v>
+      </c>
+      <c r="B3">
+        <f>(1000*Export!B3)/[1]Export!B3</f>
+        <v>5.8881256133464177</v>
+      </c>
+      <c r="C3">
+        <f>(1000*Export!C3)/[1]Export!C3</f>
+        <v>6.0367454068241466</v>
+      </c>
+      <c r="D3">
+        <f>(1000*Export!D3)/[1]Export!D3</f>
+        <v>5.7924997854629705</v>
+      </c>
+      <c r="E3">
+        <f>(1000*Export!E3)/[1]Export!E3</f>
+        <v>5.4252637874321845</v>
+      </c>
+      <c r="F3">
+        <f>(1000*Export!F3)/[1]Export!F3</f>
+        <v>5.2952202436738522</v>
+      </c>
+      <c r="G3">
+        <f>(1000*Export!G3)/[1]Export!G3</f>
+        <v>4.5435598165902462</v>
+      </c>
+      <c r="H3">
+        <f>(1000*Export!H3)/[1]Export!H3</f>
+        <v>5.1908143349528677</v>
+      </c>
+      <c r="I3">
+        <f>(1000*Export!I3)/[1]Export!I3</f>
+        <v>5.0503026173393719</v>
+      </c>
+      <c r="J3">
+        <f>(1000*Export!J3)/[1]Export!J3</f>
+        <v>4.458473071611758</v>
+      </c>
+      <c r="K3">
+        <f>(1000*Export!K3)/[1]Export!K3</f>
+        <v>5.1435919417059583</v>
+      </c>
+      <c r="L3">
+        <f>(1000*Export!L3)/[1]Export!L3</f>
+        <v>4.9539170506912447</v>
+      </c>
+      <c r="M3">
+        <f>(1000*Export!M3)/[1]Export!M3</f>
+        <v>5.11324899628816</v>
+      </c>
+      <c r="N3">
+        <f>(1000*Export!N3)/[1]Export!N3</f>
+        <v>5.6868867082961643</v>
+      </c>
+      <c r="O3">
+        <f>(1000*Export!O3)/[1]Export!O3</f>
+        <v>5.2119912763833955</v>
+      </c>
+      <c r="P3">
+        <f>(1000*Export!P3)/[1]Export!P3</f>
+        <v>5.2095130237825593</v>
+      </c>
+      <c r="Q3">
+        <f>(1000*Export!Q3)/[1]Export!Q3</f>
+        <v>4.901050755578658</v>
+      </c>
+      <c r="R3">
+        <f>(1000*Export!R3)/[1]Export!R3</f>
+        <v>4.5600955448590348</v>
+      </c>
+      <c r="S3">
+        <f>(1000*Export!S3)/[1]Export!S3</f>
+        <v>4.1067761806981515</v>
+      </c>
+      <c r="T3">
+        <f>(1000*Export!T3)/[1]Export!T3</f>
+        <v>4.4597534445250178</v>
+      </c>
+      <c r="U3">
+        <f>(1000*Export!U3)/[1]Export!U3</f>
+        <v>4.369890047927826</v>
+      </c>
+      <c r="V3">
+        <f>(1000*Export!V3)/[1]Export!V3</f>
+        <v>3.6371122701070546</v>
+      </c>
+      <c r="W3">
+        <f>(1000*Export!W3)/[1]Export!W3</f>
+        <v>2.8623383620689653</v>
+      </c>
+      <c r="X3">
+        <f>(1000*Export!X3)/[1]Export!X3</f>
+        <v>3.0021113750329902</v>
+      </c>
+      <c r="Y3">
+        <f>(1000*Export!Y3)/[1]Export!Y3</f>
+        <v>2.5263976161171211</v>
+      </c>
+      <c r="Z3">
+        <f>(1000*Export!Z3)/[1]Export!Z3</f>
+        <v>2.7436592758015634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>Export!A4</f>
+        <v>AI</v>
+      </c>
+      <c r="B4">
+        <f>(1000*Export!B4)/[1]Export!B4</f>
+        <v>5.7502246181491463</v>
+      </c>
+      <c r="C4">
+        <f>(1000*Export!C4)/[1]Export!C4</f>
+        <v>5.2530204867798984</v>
+      </c>
+      <c r="D4">
+        <f>(1000*Export!D4)/[1]Export!D4</f>
+        <v>5.0628491620111733</v>
+      </c>
+      <c r="E4">
+        <f>(1000*Export!E4)/[1]Export!E4</f>
+        <v>6.5483370670342929</v>
+      </c>
+      <c r="F4">
+        <f>(1000*Export!F4)/[1]Export!F4</f>
+        <v>5.0055617352614012</v>
+      </c>
+      <c r="G4">
+        <f>(1000*Export!G4)/[1]Export!G4</f>
+        <v>3.9467192895905279</v>
+      </c>
+      <c r="H4">
+        <f>(1000*Export!H4)/[1]Export!H4</f>
+        <v>4.8891786179921777</v>
+      </c>
+      <c r="I4">
+        <f>(1000*Export!I4)/[1]Export!I4</f>
+        <v>5.2273087280215424</v>
+      </c>
+      <c r="J4">
+        <f>(1000*Export!J4)/[1]Export!J4</f>
+        <v>6.3457669091471907</v>
+      </c>
+      <c r="K4">
+        <f>(1000*Export!K4)/[1]Export!K4</f>
+        <v>4.3426175501647197</v>
+      </c>
+      <c r="L4">
+        <f>(1000*Export!L4)/[1]Export!L4</f>
+        <v>5.7042562527424305</v>
+      </c>
+      <c r="M4">
+        <f>(1000*Export!M4)/[1]Export!M4</f>
+        <v>4.0143369175627237</v>
+      </c>
+      <c r="N4">
+        <f>(1000*Export!N4)/[1]Export!N4</f>
+        <v>5.3124563120369075</v>
+      </c>
+      <c r="O4">
+        <f>(1000*Export!O4)/[1]Export!O4</f>
+        <v>5.5789903388216082</v>
+      </c>
+      <c r="P4">
+        <f>(1000*Export!P4)/[1]Export!P4</f>
+        <v>4.1773345910254687</v>
+      </c>
+      <c r="Q4">
+        <f>(1000*Export!Q4)/[1]Export!Q4</f>
+        <v>3.66732154551408</v>
+      </c>
+      <c r="R4">
+        <f>(1000*Export!R4)/[1]Export!R4</f>
+        <v>5.5620230241883331</v>
+      </c>
+      <c r="S4">
+        <f>(1000*Export!S4)/[1]Export!S4</f>
+        <v>4.0033968215455538</v>
+      </c>
+      <c r="T4">
+        <f>(1000*Export!T4)/[1]Export!T4</f>
+        <v>4.223992276128409</v>
+      </c>
+      <c r="U4">
+        <f>(1000*Export!U4)/[1]Export!U4</f>
+        <v>5.1655318149800422</v>
+      </c>
+      <c r="V4">
+        <f>(1000*Export!V4)/[1]Export!V4</f>
+        <v>2.3110700254217704</v>
+      </c>
+      <c r="W4">
+        <f>(1000*Export!W4)/[1]Export!W4</f>
+        <v>3.0653950953678475</v>
+      </c>
+      <c r="X4">
+        <f>(1000*Export!X4)/[1]Export!X4</f>
+        <v>3.128142107027148</v>
+      </c>
+      <c r="Y4">
+        <f>(1000*Export!Y4)/[1]Export!Y4</f>
+        <v>3.2446463335496429</v>
+      </c>
+      <c r="Z4">
+        <f>(1000*Export!Z4)/[1]Export!Z4</f>
+        <v>2.9610829103214891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>Export!A5</f>
+        <v>BL</v>
+      </c>
+      <c r="B5">
+        <f>(1000*Export!B5)/[1]Export!B5</f>
+        <v>5.7323759399998</v>
+      </c>
+      <c r="C5">
+        <f>(1000*Export!C5)/[1]Export!C5</f>
+        <v>5.4540604096473633</v>
+      </c>
+      <c r="D5">
+        <f>(1000*Export!D5)/[1]Export!D5</f>
+        <v>6.1168185283333942</v>
+      </c>
+      <c r="E5">
+        <f>(1000*Export!E5)/[1]Export!E5</f>
+        <v>6.4543736404806902</v>
+      </c>
+      <c r="F5">
+        <f>(1000*Export!F5)/[1]Export!F5</f>
+        <v>5.6014514452801603</v>
+      </c>
+      <c r="G5">
+        <f>(1000*Export!G5)/[1]Export!G5</f>
+        <v>6.1302549668016475</v>
+      </c>
+      <c r="H5">
+        <f>(1000*Export!H5)/[1]Export!H5</f>
+        <v>6.3431732758984758</v>
+      </c>
+      <c r="I5">
+        <f>(1000*Export!I5)/[1]Export!I5</f>
+        <v>5.9817667193259609</v>
+      </c>
+      <c r="J5">
+        <f>(1000*Export!J5)/[1]Export!J5</f>
+        <v>6.1270272660754062</v>
+      </c>
+      <c r="K5">
+        <f>(1000*Export!K5)/[1]Export!K5</f>
+        <v>5.5807876073455445</v>
+      </c>
+      <c r="L5">
+        <f>(1000*Export!L5)/[1]Export!L5</f>
+        <v>5.1048383982700702</v>
+      </c>
+      <c r="M5">
+        <f>(1000*Export!M5)/[1]Export!M5</f>
+        <v>5.5579632459721875</v>
+      </c>
+      <c r="N5">
+        <f>(1000*Export!N5)/[1]Export!N5</f>
+        <v>5.0224390831601458</v>
+      </c>
+      <c r="O5">
+        <f>(1000*Export!O5)/[1]Export!O5</f>
+        <v>4.9102785494406485</v>
+      </c>
+      <c r="P5">
+        <f>(1000*Export!P5)/[1]Export!P5</f>
+        <v>5.2044278470299128</v>
+      </c>
+      <c r="Q5">
+        <f>(1000*Export!Q5)/[1]Export!Q5</f>
+        <v>5.0969537330535593</v>
+      </c>
+      <c r="R5">
+        <f>(1000*Export!R5)/[1]Export!R5</f>
+        <v>5.2779345682722827</v>
+      </c>
+      <c r="S5">
+        <f>(1000*Export!S5)/[1]Export!S5</f>
+        <v>5.1435440136415735</v>
+      </c>
+      <c r="T5">
+        <f>(1000*Export!T5)/[1]Export!T5</f>
+        <v>4.4212887586381564</v>
+      </c>
+      <c r="U5">
+        <f>(1000*Export!U5)/[1]Export!U5</f>
+        <v>3.8889921505268727</v>
+      </c>
+      <c r="V5">
+        <f>(1000*Export!V5)/[1]Export!V5</f>
+        <v>3.4054458873235456</v>
+      </c>
+      <c r="W5">
+        <f>(1000*Export!W5)/[1]Export!W5</f>
+        <v>3.2976614025959416</v>
+      </c>
+      <c r="X5">
+        <f>(1000*Export!X5)/[1]Export!X5</f>
+        <v>3.3078915847238086</v>
+      </c>
+      <c r="Y5">
+        <f>(1000*Export!Y5)/[1]Export!Y5</f>
+        <v>3.2964835210305994</v>
+      </c>
+      <c r="Z5">
+        <f>(1000*Export!Z5)/[1]Export!Z5</f>
+        <v>3.4508391813463728</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>Export!A6</f>
+        <v>BS</v>
+      </c>
+      <c r="B6">
+        <f>(1000*Export!B6)/[1]Export!B6</f>
+        <v>11.347077972407378</v>
+      </c>
+      <c r="C6">
+        <f>(1000*Export!C6)/[1]Export!C6</f>
+        <v>12.281714758345167</v>
+      </c>
+      <c r="D6">
+        <f>(1000*Export!D6)/[1]Export!D6</f>
+        <v>13.506964528585051</v>
+      </c>
+      <c r="E6">
+        <f>(1000*Export!E6)/[1]Export!E6</f>
+        <v>13.432275032876198</v>
+      </c>
+      <c r="F6">
+        <f>(1000*Export!F6)/[1]Export!F6</f>
+        <v>12.316623519259434</v>
+      </c>
+      <c r="G6">
+        <f>(1000*Export!G6)/[1]Export!G6</f>
+        <v>12.966271880583799</v>
+      </c>
+      <c r="H6">
+        <f>(1000*Export!H6)/[1]Export!H6</f>
+        <v>11.432265796237601</v>
+      </c>
+      <c r="I6">
+        <f>(1000*Export!I6)/[1]Export!I6</f>
+        <v>11.503235284923885</v>
+      </c>
+      <c r="J6">
+        <f>(1000*Export!J6)/[1]Export!J6</f>
+        <v>10.305415027168822</v>
+      </c>
+      <c r="K6">
+        <f>(1000*Export!K6)/[1]Export!K6</f>
+        <v>9.3390027058368759</v>
+      </c>
+      <c r="L6">
+        <f>(1000*Export!L6)/[1]Export!L6</f>
+        <v>8.822075273468883</v>
+      </c>
+      <c r="M6">
+        <f>(1000*Export!M6)/[1]Export!M6</f>
+        <v>8.8152165609961042</v>
+      </c>
+      <c r="N6">
+        <f>(1000*Export!N6)/[1]Export!N6</f>
+        <v>8.0966693246641714</v>
+      </c>
+      <c r="O6">
+        <f>(1000*Export!O6)/[1]Export!O6</f>
+        <v>9.1582552543037767</v>
+      </c>
+      <c r="P6">
+        <f>(1000*Export!P6)/[1]Export!P6</f>
+        <v>8.8255261371350979</v>
+      </c>
+      <c r="Q6">
+        <f>(1000*Export!Q6)/[1]Export!Q6</f>
+        <v>8.1761978361669243</v>
+      </c>
+      <c r="R6">
+        <f>(1000*Export!R6)/[1]Export!R6</f>
+        <v>7.5781931750332978</v>
+      </c>
+      <c r="S6">
+        <f>(1000*Export!S6)/[1]Export!S6</f>
+        <v>7.3361413761482153</v>
+      </c>
+      <c r="T6">
+        <f>(1000*Export!T6)/[1]Export!T6</f>
+        <v>5.7660002724094621</v>
+      </c>
+      <c r="U6">
+        <f>(1000*Export!U6)/[1]Export!U6</f>
+        <v>4.7652691550290873</v>
+      </c>
+      <c r="V6">
+        <f>(1000*Export!V6)/[1]Export!V6</f>
+        <v>3.8007007542015558</v>
+      </c>
+      <c r="W6">
+        <f>(1000*Export!W6)/[1]Export!W6</f>
+        <v>4.8948432003592544</v>
+      </c>
+      <c r="X6">
+        <f>(1000*Export!X6)/[1]Export!X6</f>
+        <v>5.5797577131944855</v>
+      </c>
+      <c r="Y6">
+        <f>(1000*Export!Y6)/[1]Export!Y6</f>
+        <v>5.9475821785491547</v>
+      </c>
+      <c r="Z6">
+        <f>(1000*Export!Z6)/[1]Export!Z6</f>
+        <v>6.2617502577475896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>Export!A7</f>
+        <v>BE</v>
+      </c>
+      <c r="B7">
+        <f>(1000*Export!B7)/[1]Export!B7</f>
+        <v>8.2250884254177343</v>
+      </c>
+      <c r="C7">
+        <f>(1000*Export!C7)/[1]Export!C7</f>
+        <v>8.0614047556196322</v>
+      </c>
+      <c r="D7">
+        <f>(1000*Export!D7)/[1]Export!D7</f>
+        <v>8.2618025751072963</v>
+      </c>
+      <c r="E7">
+        <f>(1000*Export!E7)/[1]Export!E7</f>
+        <v>7.9411316112546038</v>
+      </c>
+      <c r="F7">
+        <f>(1000*Export!F7)/[1]Export!F7</f>
+        <v>7.6195620076877066</v>
+      </c>
+      <c r="G7">
+        <f>(1000*Export!G7)/[1]Export!G7</f>
+        <v>7.5875433281476026</v>
+      </c>
+      <c r="H7">
+        <f>(1000*Export!H7)/[1]Export!H7</f>
+        <v>7.3489305333696961</v>
+      </c>
+      <c r="I7">
+        <f>(1000*Export!I7)/[1]Export!I7</f>
+        <v>7.3976014342822998</v>
+      </c>
+      <c r="J7">
+        <f>(1000*Export!J7)/[1]Export!J7</f>
+        <v>7.1106659989984982</v>
+      </c>
+      <c r="K7">
+        <f>(1000*Export!K7)/[1]Export!K7</f>
+        <v>7.1830902542199233</v>
+      </c>
+      <c r="L7">
+        <f>(1000*Export!L7)/[1]Export!L7</f>
+        <v>7.2273646511710776</v>
+      </c>
+      <c r="M7">
+        <f>(1000*Export!M7)/[1]Export!M7</f>
+        <v>7.2813989763480675</v>
+      </c>
+      <c r="N7">
+        <f>(1000*Export!N7)/[1]Export!N7</f>
+        <v>6.9152427809154897</v>
+      </c>
+      <c r="O7">
+        <f>(1000*Export!O7)/[1]Export!O7</f>
+        <v>6.4212908341875714</v>
+      </c>
+      <c r="P7">
+        <f>(1000*Export!P7)/[1]Export!P7</f>
+        <v>6.0558568159734198</v>
+      </c>
+      <c r="Q7">
+        <f>(1000*Export!Q7)/[1]Export!Q7</f>
+        <v>6.0154969174474342</v>
+      </c>
+      <c r="R7">
+        <f>(1000*Export!R7)/[1]Export!R7</f>
+        <v>5.6095913334688507</v>
+      </c>
+      <c r="S7">
+        <f>(1000*Export!S7)/[1]Export!S7</f>
+        <v>5.3753974803089477</v>
+      </c>
+      <c r="T7">
+        <f>(1000*Export!T7)/[1]Export!T7</f>
+        <v>5.3244350194390737</v>
+      </c>
+      <c r="U7">
+        <f>(1000*Export!U7)/[1]Export!U7</f>
+        <v>5.3852832290403958</v>
+      </c>
+      <c r="V7">
+        <f>(1000*Export!V7)/[1]Export!V7</f>
+        <v>5.2248749129522958</v>
+      </c>
+      <c r="W7">
+        <f>(1000*Export!W7)/[1]Export!W7</f>
+        <v>4.8772660368350467</v>
+      </c>
+      <c r="X7">
+        <f>(1000*Export!X7)/[1]Export!X7</f>
+        <v>4.8999791033174951</v>
+      </c>
+      <c r="Y7">
+        <f>(1000*Export!Y7)/[1]Export!Y7</f>
+        <v>4.9074113260975789</v>
+      </c>
+      <c r="Z7">
+        <f>(1000*Export!Z7)/[1]Export!Z7</f>
+        <v>4.6746340889868279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>Export!A8</f>
+        <v>FR</v>
+      </c>
+      <c r="B8">
+        <f>(1000*Export!B8)/[1]Export!B8</f>
+        <v>5.9658751938909438</v>
+      </c>
+      <c r="C8">
+        <f>(1000*Export!C8)/[1]Export!C8</f>
+        <v>5.5971789436667869</v>
+      </c>
+      <c r="D8">
+        <f>(1000*Export!D8)/[1]Export!D8</f>
+        <v>6.069023248734827</v>
+      </c>
+      <c r="E8">
+        <f>(1000*Export!E8)/[1]Export!E8</f>
+        <v>5.9039087947882738</v>
+      </c>
+      <c r="F8">
+        <f>(1000*Export!F8)/[1]Export!F8</f>
+        <v>5.0033415819229452</v>
+      </c>
+      <c r="G8">
+        <f>(1000*Export!G8)/[1]Export!G8</f>
+        <v>5.2803065756593757</v>
+      </c>
+      <c r="H8">
+        <f>(1000*Export!H8)/[1]Export!H8</f>
+        <v>5.1510306382610951</v>
+      </c>
+      <c r="I8">
+        <f>(1000*Export!I8)/[1]Export!I8</f>
+        <v>5.6225506239352816</v>
+      </c>
+      <c r="J8">
+        <f>(1000*Export!J8)/[1]Export!J8</f>
+        <v>5.3690396294053135</v>
+      </c>
+      <c r="K8">
+        <f>(1000*Export!K8)/[1]Export!K8</f>
+        <v>5.4233994600492164</v>
+      </c>
+      <c r="L8">
+        <f>(1000*Export!L8)/[1]Export!L8</f>
+        <v>5.012959197926528</v>
+      </c>
+      <c r="M8">
+        <f>(1000*Export!M8)/[1]Export!M8</f>
+        <v>5.5923652057625679</v>
+      </c>
+      <c r="N8">
+        <f>(1000*Export!N8)/[1]Export!N8</f>
+        <v>5.5885876723643966</v>
+      </c>
+      <c r="O8">
+        <f>(1000*Export!O8)/[1]Export!O8</f>
+        <v>5.3921353732848187</v>
+      </c>
+      <c r="P8">
+        <f>(1000*Export!P8)/[1]Export!P8</f>
+        <v>4.9937045178087454</v>
+      </c>
+      <c r="Q8">
+        <f>(1000*Export!Q8)/[1]Export!Q8</f>
+        <v>4.7903772859190878</v>
+      </c>
+      <c r="R8">
+        <f>(1000*Export!R8)/[1]Export!R8</f>
+        <v>4.1428610110747073</v>
+      </c>
+      <c r="S8">
+        <f>(1000*Export!S8)/[1]Export!S8</f>
+        <v>3.9534584726150683</v>
+      </c>
+      <c r="T8">
+        <f>(1000*Export!T8)/[1]Export!T8</f>
+        <v>4.0926190167336882</v>
+      </c>
+      <c r="U8">
+        <f>(1000*Export!U8)/[1]Export!U8</f>
+        <v>3.8073781324338269</v>
+      </c>
+      <c r="V8">
+        <f>(1000*Export!V8)/[1]Export!V8</f>
+        <v>3.1970866928117312</v>
+      </c>
+      <c r="W8">
+        <f>(1000*Export!W8)/[1]Export!W8</f>
+        <v>3.2254040665039114</v>
+      </c>
+      <c r="X8">
+        <f>(1000*Export!X8)/[1]Export!X8</f>
+        <v>3.1932187645146306</v>
+      </c>
+      <c r="Y8">
+        <f>(1000*Export!Y8)/[1]Export!Y8</f>
+        <v>3.0647737959007944</v>
+      </c>
+      <c r="Z8">
+        <f>(1000*Export!Z8)/[1]Export!Z8</f>
+        <v>3.0511652677536212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>Export!A9</f>
+        <v>GE</v>
+      </c>
+      <c r="B9">
+        <f>(1000*Export!B9)/[1]Export!B9</f>
+        <v>5.8220084372421734</v>
+      </c>
+      <c r="C9">
+        <f>(1000*Export!C9)/[1]Export!C9</f>
+        <v>5.6482750355622482</v>
+      </c>
+      <c r="D9">
+        <f>(1000*Export!D9)/[1]Export!D9</f>
+        <v>5.7913865351550031</v>
+      </c>
+      <c r="E9">
+        <f>(1000*Export!E9)/[1]Export!E9</f>
+        <v>5.2678544267215592</v>
+      </c>
+      <c r="F9">
+        <f>(1000*Export!F9)/[1]Export!F9</f>
+        <v>5.166136550041009</v>
+      </c>
+      <c r="G9">
+        <f>(1000*Export!G9)/[1]Export!G9</f>
+        <v>5.1428260299263968</v>
+      </c>
+      <c r="H9">
+        <f>(1000*Export!H9)/[1]Export!H9</f>
+        <v>5.7139499698879241</v>
+      </c>
+      <c r="I9">
+        <f>(1000*Export!I9)/[1]Export!I9</f>
+        <v>5.8892701546053896</v>
+      </c>
+      <c r="J9">
+        <f>(1000*Export!J9)/[1]Export!J9</f>
+        <v>5.8994279057970331</v>
+      </c>
+      <c r="K9">
+        <f>(1000*Export!K9)/[1]Export!K9</f>
+        <v>6.2404716859835059</v>
+      </c>
+      <c r="L9">
+        <f>(1000*Export!L9)/[1]Export!L9</f>
+        <v>6.1579142782109448</v>
+      </c>
+      <c r="M9">
+        <f>(1000*Export!M9)/[1]Export!M9</f>
+        <v>6.0622959371823812</v>
+      </c>
+      <c r="N9">
+        <f>(1000*Export!N9)/[1]Export!N9</f>
+        <v>5.8978188354602441</v>
+      </c>
+      <c r="O9">
+        <f>(1000*Export!O9)/[1]Export!O9</f>
+        <v>5.4563094697677732</v>
+      </c>
+      <c r="P9">
+        <f>(1000*Export!P9)/[1]Export!P9</f>
+        <v>5.3612320955502675</v>
+      </c>
+      <c r="Q9">
+        <f>(1000*Export!Q9)/[1]Export!Q9</f>
+        <v>5.3920660245603411</v>
+      </c>
+      <c r="R9">
+        <f>(1000*Export!R9)/[1]Export!R9</f>
+        <v>5.6866726075093474</v>
+      </c>
+      <c r="S9">
+        <f>(1000*Export!S9)/[1]Export!S9</f>
+        <v>5.3114055690692021</v>
+      </c>
+      <c r="T9">
+        <f>(1000*Export!T9)/[1]Export!T9</f>
+        <v>5.1176883567971032</v>
+      </c>
+      <c r="U9">
+        <f>(1000*Export!U9)/[1]Export!U9</f>
+        <v>4.2058001557703761</v>
+      </c>
+      <c r="V9">
+        <f>(1000*Export!V9)/[1]Export!V9</f>
+        <v>4.6549511753410444</v>
+      </c>
+      <c r="W9">
+        <f>(1000*Export!W9)/[1]Export!W9</f>
+        <v>5.3859309086763201</v>
+      </c>
+      <c r="X9">
+        <f>(1000*Export!X9)/[1]Export!X9</f>
+        <v>5.918883971662205</v>
+      </c>
+      <c r="Y9">
+        <f>(1000*Export!Y9)/[1]Export!Y9</f>
+        <v>5.7157585815513041</v>
+      </c>
+      <c r="Z9">
+        <f>(1000*Export!Z9)/[1]Export!Z9</f>
+        <v>5.2760454010470923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>Export!A10</f>
+        <v>GL</v>
+      </c>
+      <c r="B10">
+        <f>(1000*Export!B10)/[1]Export!B10</f>
+        <v>6.8429237947122861</v>
+      </c>
+      <c r="C10">
+        <f>(1000*Export!C10)/[1]Export!C10</f>
+        <v>6.0711188204683433</v>
+      </c>
+      <c r="D10">
+        <f>(1000*Export!D10)/[1]Export!D10</f>
+        <v>6.6967003530987457</v>
+      </c>
+      <c r="E10">
+        <f>(1000*Export!E10)/[1]Export!E10</f>
+        <v>4.8369759942672879</v>
+      </c>
+      <c r="F10">
+        <f>(1000*Export!F10)/[1]Export!F10</f>
+        <v>5.7183702644746246</v>
+      </c>
+      <c r="G10">
+        <f>(1000*Export!G10)/[1]Export!G10</f>
+        <v>5.1062331259537501</v>
+      </c>
+      <c r="H10">
+        <f>(1000*Export!H10)/[1]Export!H10</f>
+        <v>4.9099836333878883</v>
+      </c>
+      <c r="I10">
+        <f>(1000*Export!I10)/[1]Export!I10</f>
+        <v>5.7839880884205703</v>
+      </c>
+      <c r="J10">
+        <f>(1000*Export!J10)/[1]Export!J10</f>
+        <v>5.7107316521542462</v>
+      </c>
+      <c r="K10">
+        <f>(1000*Export!K10)/[1]Export!K10</f>
+        <v>4.7719454000665849</v>
+      </c>
+      <c r="L10">
+        <f>(1000*Export!L10)/[1]Export!L10</f>
+        <v>5.9630292188431726</v>
+      </c>
+      <c r="M10">
+        <f>(1000*Export!M10)/[1]Export!M10</f>
+        <v>5.5313264546324863</v>
+      </c>
+      <c r="N10">
+        <f>(1000*Export!N10)/[1]Export!N10</f>
+        <v>5.2254794377384126</v>
+      </c>
+      <c r="O10">
+        <f>(1000*Export!O10)/[1]Export!O10</f>
+        <v>5.8524963745597676</v>
+      </c>
+      <c r="P10">
+        <f>(1000*Export!P10)/[1]Export!P10</f>
+        <v>4.6880051729712253</v>
+      </c>
+      <c r="Q10">
+        <f>(1000*Export!Q10)/[1]Export!Q10</f>
+        <v>5.5017722054700311</v>
+      </c>
+      <c r="R10">
+        <f>(1000*Export!R10)/[1]Export!R10</f>
+        <v>5.4837859214342206</v>
+      </c>
+      <c r="S10">
+        <f>(1000*Export!S10)/[1]Export!S10</f>
+        <v>5.9859330573153091</v>
+      </c>
+      <c r="T10">
+        <f>(1000*Export!T10)/[1]Export!T10</f>
+        <v>3.9707520216938645</v>
+      </c>
+      <c r="U10">
+        <f>(1000*Export!U10)/[1]Export!U10</f>
+        <v>4.048582995951417</v>
+      </c>
+      <c r="V10">
+        <f>(1000*Export!V10)/[1]Export!V10</f>
+        <v>3.7118504261754195</v>
+      </c>
+      <c r="W10">
+        <f>(1000*Export!W10)/[1]Export!W10</f>
+        <v>4.184476940382452</v>
+      </c>
+      <c r="X10">
+        <f>(1000*Export!X10)/[1]Export!X10</f>
+        <v>3.9872408293460926</v>
+      </c>
+      <c r="Y10">
+        <f>(1000*Export!Y10)/[1]Export!Y10</f>
+        <v>4.5626385086690133</v>
+      </c>
+      <c r="Z10">
+        <f>(1000*Export!Z10)/[1]Export!Z10</f>
+        <v>4.3045930007317805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>Export!A11</f>
+        <v>GR</v>
+      </c>
+      <c r="B11">
+        <f>(1000*Export!B11)/[1]Export!B11</f>
+        <v>10.692883161646625</v>
+      </c>
+      <c r="C11">
+        <f>(1000*Export!C11)/[1]Export!C11</f>
+        <v>10.7488217390746</v>
+      </c>
+      <c r="D11">
+        <f>(1000*Export!D11)/[1]Export!D11</f>
+        <v>9.86433403195241</v>
+      </c>
+      <c r="E11">
+        <f>(1000*Export!E11)/[1]Export!E11</f>
+        <v>9.5565655324898664</v>
+      </c>
+      <c r="F11">
+        <f>(1000*Export!F11)/[1]Export!F11</f>
+        <v>9.0596385834019664</v>
+      </c>
+      <c r="G11">
+        <f>(1000*Export!G11)/[1]Export!G11</f>
+        <v>8.8491290084375418</v>
+      </c>
+      <c r="H11">
+        <f>(1000*Export!H11)/[1]Export!H11</f>
+        <v>9.0486349145473284</v>
+      </c>
+      <c r="I11">
+        <f>(1000*Export!I11)/[1]Export!I11</f>
+        <v>8.8455966360820248</v>
+      </c>
+      <c r="J11">
+        <f>(1000*Export!J11)/[1]Export!J11</f>
+        <v>8.0974961842733801</v>
+      </c>
+      <c r="K11">
+        <f>(1000*Export!K11)/[1]Export!K11</f>
+        <v>8.8811172721625287</v>
+      </c>
+      <c r="L11">
+        <f>(1000*Export!L11)/[1]Export!L11</f>
+        <v>7.9920193168807323</v>
+      </c>
+      <c r="M11">
+        <f>(1000*Export!M11)/[1]Export!M11</f>
+        <v>8.1336238198983288</v>
+      </c>
+      <c r="N11">
+        <f>(1000*Export!N11)/[1]Export!N11</f>
+        <v>7.6229083818944909</v>
+      </c>
+      <c r="O11">
+        <f>(1000*Export!O11)/[1]Export!O11</f>
+        <v>7.219433935675494</v>
+      </c>
+      <c r="P11">
+        <f>(1000*Export!P11)/[1]Export!P11</f>
+        <v>6.6284257488846396</v>
+      </c>
+      <c r="Q11">
+        <f>(1000*Export!Q11)/[1]Export!Q11</f>
+        <v>7.1649398395721926</v>
+      </c>
+      <c r="R11">
+        <f>(1000*Export!R11)/[1]Export!R11</f>
+        <v>6.2283030426791912</v>
+      </c>
+      <c r="S11">
+        <f>(1000*Export!S11)/[1]Export!S11</f>
+        <v>5.6021854461952652</v>
+      </c>
+      <c r="T11">
+        <f>(1000*Export!T11)/[1]Export!T11</f>
+        <v>5.6231397694812326</v>
+      </c>
+      <c r="U11">
+        <f>(1000*Export!U11)/[1]Export!U11</f>
+        <v>5.1413379207882084</v>
+      </c>
+      <c r="V11">
+        <f>(1000*Export!V11)/[1]Export!V11</f>
+        <v>4.7829497407641242</v>
+      </c>
+      <c r="W11">
+        <f>(1000*Export!W11)/[1]Export!W11</f>
+        <v>4.6978472916627361</v>
+      </c>
+      <c r="X11">
+        <f>(1000*Export!X11)/[1]Export!X11</f>
+        <v>4.8856606787910311</v>
+      </c>
+      <c r="Y11">
+        <f>(1000*Export!Y11)/[1]Export!Y11</f>
+        <v>4.4205670773004337</v>
+      </c>
+      <c r="Z11">
+        <f>(1000*Export!Z11)/[1]Export!Z11</f>
+        <v>4.4434008272673085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>Export!A12</f>
+        <v>JU</v>
+      </c>
+      <c r="B12">
+        <f>(1000*Export!B12)/[1]Export!B12</f>
+        <v>7.4403773334219094</v>
+      </c>
+      <c r="C12">
+        <f>(1000*Export!C12)/[1]Export!C12</f>
+        <v>8.1674492427749481</v>
+      </c>
+      <c r="D12">
+        <f>(1000*Export!D12)/[1]Export!D12</f>
+        <v>6.3575047600606709</v>
+      </c>
+      <c r="E12">
+        <f>(1000*Export!E12)/[1]Export!E12</f>
+        <v>6.935607024688216</v>
+      </c>
+      <c r="F12">
+        <f>(1000*Export!F12)/[1]Export!F12</f>
+        <v>6.6072430343451973</v>
+      </c>
+      <c r="G12">
+        <f>(1000*Export!G12)/[1]Export!G12</f>
+        <v>5.8323207776427708</v>
+      </c>
+      <c r="H12">
+        <f>(1000*Export!H12)/[1]Export!H12</f>
+        <v>6.35384661277332</v>
+      </c>
+      <c r="I12">
+        <f>(1000*Export!I12)/[1]Export!I12</f>
+        <v>6.6271567453945641</v>
+      </c>
+      <c r="J12">
+        <f>(1000*Export!J12)/[1]Export!J12</f>
+        <v>6.2762111352133045</v>
+      </c>
+      <c r="K12">
+        <f>(1000*Export!K12)/[1]Export!K12</f>
+        <v>5.7818285388778126</v>
+      </c>
+      <c r="L12">
+        <f>(1000*Export!L12)/[1]Export!L12</f>
+        <v>6.2066241606951422</v>
+      </c>
+      <c r="M12">
+        <f>(1000*Export!M12)/[1]Export!M12</f>
+        <v>4.7757878661668753</v>
+      </c>
+      <c r="N12">
+        <f>(1000*Export!N12)/[1]Export!N12</f>
+        <v>4.990129414345251</v>
+      </c>
+      <c r="O12">
+        <f>(1000*Export!O12)/[1]Export!O12</f>
+        <v>4.3886977487605989</v>
+      </c>
+      <c r="P12">
+        <f>(1000*Export!P12)/[1]Export!P12</f>
+        <v>4.5158324545036637</v>
+      </c>
+      <c r="Q12">
+        <f>(1000*Export!Q12)/[1]Export!Q12</f>
+        <v>4.5541706615532123</v>
+      </c>
+      <c r="R12">
+        <f>(1000*Export!R12)/[1]Export!R12</f>
+        <v>4.2229729729729728</v>
+      </c>
+      <c r="S12">
+        <f>(1000*Export!S12)/[1]Export!S12</f>
+        <v>4.2062379302134865</v>
+      </c>
+      <c r="T12">
+        <f>(1000*Export!T12)/[1]Export!T12</f>
+        <v>4.0155440414507773</v>
+      </c>
+      <c r="U12">
+        <f>(1000*Export!U12)/[1]Export!U12</f>
+        <v>3.7805744443316756</v>
+      </c>
+      <c r="V12">
+        <f>(1000*Export!V12)/[1]Export!V12</f>
+        <v>3.6679392170072611</v>
+      </c>
+      <c r="W12">
+        <f>(1000*Export!W12)/[1]Export!W12</f>
+        <v>2.8088515460895902</v>
+      </c>
+      <c r="X12">
+        <f>(1000*Export!X12)/[1]Export!X12</f>
+        <v>3.8853226507070806</v>
+      </c>
+      <c r="Y12">
+        <f>(1000*Export!Y12)/[1]Export!Y12</f>
+        <v>3.9296006096834883</v>
+      </c>
+      <c r="Z12">
+        <f>(1000*Export!Z12)/[1]Export!Z12</f>
+        <v>3.1473869641808574</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>Export!A13</f>
+        <v>LU</v>
+      </c>
+      <c r="B13">
+        <f>(1000*Export!B13)/[1]Export!B13</f>
+        <v>8.2981008238024074</v>
+      </c>
+      <c r="C13">
+        <f>(1000*Export!C13)/[1]Export!C13</f>
+        <v>7.826891067135195</v>
+      </c>
+      <c r="D13">
+        <f>(1000*Export!D13)/[1]Export!D13</f>
+        <v>7.6719288695336596</v>
+      </c>
+      <c r="E13">
+        <f>(1000*Export!E13)/[1]Export!E13</f>
+        <v>7.7052165530046057</v>
+      </c>
+      <c r="F13">
+        <f>(1000*Export!F13)/[1]Export!F13</f>
+        <v>7.2608280433683499</v>
+      </c>
+      <c r="G13">
+        <f>(1000*Export!G13)/[1]Export!G13</f>
+        <v>7.9177442055562874</v>
+      </c>
+      <c r="H13">
+        <f>(1000*Export!H13)/[1]Export!H13</f>
+        <v>7.379772343554273</v>
+      </c>
+      <c r="I13">
+        <f>(1000*Export!I13)/[1]Export!I13</f>
+        <v>7.738601339143373</v>
+      </c>
+      <c r="J13">
+        <f>(1000*Export!J13)/[1]Export!J13</f>
+        <v>7.6954993970670227</v>
+      </c>
+      <c r="K13">
+        <f>(1000*Export!K13)/[1]Export!K13</f>
+        <v>8.2865425790600593</v>
+      </c>
+      <c r="L13">
+        <f>(1000*Export!L13)/[1]Export!L13</f>
+        <v>7.6681899979592716</v>
+      </c>
+      <c r="M13">
+        <f>(1000*Export!M13)/[1]Export!M13</f>
+        <v>7.941262776935492</v>
+      </c>
+      <c r="N13">
+        <f>(1000*Export!N13)/[1]Export!N13</f>
+        <v>7.1107694525187979</v>
+      </c>
+      <c r="O13">
+        <f>(1000*Export!O13)/[1]Export!O13</f>
+        <v>7.1662086610442532</v>
+      </c>
+      <c r="P13">
+        <f>(1000*Export!P13)/[1]Export!P13</f>
+        <v>6.5240860152306483</v>
+      </c>
+      <c r="Q13">
+        <f>(1000*Export!Q13)/[1]Export!Q13</f>
+        <v>6.3022214617731773</v>
+      </c>
+      <c r="R13">
+        <f>(1000*Export!R13)/[1]Export!R13</f>
+        <v>6.3482652735906573</v>
+      </c>
+      <c r="S13">
+        <f>(1000*Export!S13)/[1]Export!S13</f>
+        <v>6.4134955494227857</v>
+      </c>
+      <c r="T13">
+        <f>(1000*Export!T13)/[1]Export!T13</f>
+        <v>5.8913093771352631</v>
+      </c>
+      <c r="U13">
+        <f>(1000*Export!U13)/[1]Export!U13</f>
+        <v>5.796479175611851</v>
+      </c>
+      <c r="V13">
+        <f>(1000*Export!V13)/[1]Export!V13</f>
+        <v>5.2556188223539664</v>
+      </c>
+      <c r="W13">
+        <f>(1000*Export!W13)/[1]Export!W13</f>
+        <v>4.832076593660835</v>
+      </c>
+      <c r="X13">
+        <f>(1000*Export!X13)/[1]Export!X13</f>
+        <v>4.9440490293020574</v>
+      </c>
+      <c r="Y13">
+        <f>(1000*Export!Y13)/[1]Export!Y13</f>
+        <v>4.8454525451779853</v>
+      </c>
+      <c r="Z13">
+        <f>(1000*Export!Z13)/[1]Export!Z13</f>
+        <v>4.0129352626712533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" t="str">
+        <f>Export!A14</f>
+        <v>NE</v>
+      </c>
+      <c r="B14">
+        <f>(1000*Export!B14)/[1]Export!B14</f>
+        <v>7.4438441109904634</v>
+      </c>
+      <c r="C14">
+        <f>(1000*Export!C14)/[1]Export!C14</f>
+        <v>6.7745183945176102</v>
+      </c>
+      <c r="D14">
+        <f>(1000*Export!D14)/[1]Export!D14</f>
+        <v>6.9772850608574304</v>
+      </c>
+      <c r="E14">
+        <f>(1000*Export!E14)/[1]Export!E14</f>
+        <v>6.1552128942191766</v>
+      </c>
+      <c r="F14">
+        <f>(1000*Export!F14)/[1]Export!F14</f>
+        <v>5.8234623581305449</v>
+      </c>
+      <c r="G14">
+        <f>(1000*Export!G14)/[1]Export!G14</f>
+        <v>5.5825391945896099</v>
+      </c>
+      <c r="H14">
+        <f>(1000*Export!H14)/[1]Export!H14</f>
+        <v>5.8189181935735723</v>
+      </c>
+      <c r="I14">
+        <f>(1000*Export!I14)/[1]Export!I14</f>
+        <v>5.7683738966028013</v>
+      </c>
+      <c r="J14">
+        <f>(1000*Export!J14)/[1]Export!J14</f>
+        <v>6.0901339829476244</v>
+      </c>
+      <c r="K14">
+        <f>(1000*Export!K14)/[1]Export!K14</f>
+        <v>6.1119988802444798</v>
+      </c>
+      <c r="L14">
+        <f>(1000*Export!L14)/[1]Export!L14</f>
+        <v>5.9157240407168192</v>
+      </c>
+      <c r="M14">
+        <f>(1000*Export!M14)/[1]Export!M14</f>
+        <v>5.1491885430554918</v>
+      </c>
+      <c r="N14">
+        <f>(1000*Export!N14)/[1]Export!N14</f>
+        <v>5.079958084650781</v>
+      </c>
+      <c r="O14">
+        <f>(1000*Export!O14)/[1]Export!O14</f>
+        <v>4.6276244101488588</v>
+      </c>
+      <c r="P14">
+        <f>(1000*Export!P14)/[1]Export!P14</f>
+        <v>4.8910166409648541</v>
+      </c>
+      <c r="Q14">
+        <f>(1000*Export!Q14)/[1]Export!Q14</f>
+        <v>4.3880197917976025</v>
+      </c>
+      <c r="R14">
+        <f>(1000*Export!R14)/[1]Export!R14</f>
+        <v>4.2557054824835161</v>
+      </c>
+      <c r="S14">
+        <f>(1000*Export!S14)/[1]Export!S14</f>
+        <v>4.077898018661184</v>
+      </c>
+      <c r="T14">
+        <f>(1000*Export!T14)/[1]Export!T14</f>
+        <v>3.411869304289842</v>
+      </c>
+      <c r="U14">
+        <f>(1000*Export!U14)/[1]Export!U14</f>
+        <v>3.3801096900112308</v>
+      </c>
+      <c r="V14">
+        <f>(1000*Export!V14)/[1]Export!V14</f>
+        <v>3.1651999101767592</v>
+      </c>
+      <c r="W14">
+        <f>(1000*Export!W14)/[1]Export!W14</f>
+        <v>2.9507851196121826</v>
+      </c>
+      <c r="X14">
+        <f>(1000*Export!X14)/[1]Export!X14</f>
+        <v>2.9939805233688057</v>
+      </c>
+      <c r="Y14">
+        <f>(1000*Export!Y14)/[1]Export!Y14</f>
+        <v>2.9297179367305595</v>
+      </c>
+      <c r="Z14">
+        <f>(1000*Export!Z14)/[1]Export!Z14</f>
+        <v>3.0947616001980647</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A15" t="str">
+        <f>Export!A15</f>
+        <v>NW</v>
+      </c>
+      <c r="B15">
+        <f>(1000*Export!B15)/[1]Export!B15</f>
+        <v>6.3544944166820905</v>
+      </c>
+      <c r="C15">
+        <f>(1000*Export!C15)/[1]Export!C15</f>
+        <v>4.9742189869578404</v>
+      </c>
+      <c r="D15">
+        <f>(1000*Export!D15)/[1]Export!D15</f>
+        <v>6.742243436754177</v>
+      </c>
+      <c r="E15">
+        <f>(1000*Export!E15)/[1]Export!E15</f>
+        <v>6.2977433086477346</v>
+      </c>
+      <c r="F15">
+        <f>(1000*Export!F15)/[1]Export!F15</f>
+        <v>6.9121605089307563</v>
+      </c>
+      <c r="G15">
+        <f>(1000*Export!G15)/[1]Export!G15</f>
+        <v>4.4876993782103272</v>
+      </c>
+      <c r="H15">
+        <f>(1000*Export!H15)/[1]Export!H15</f>
+        <v>5.2223538279315171</v>
+      </c>
+      <c r="I15">
+        <f>(1000*Export!I15)/[1]Export!I15</f>
+        <v>6.6018609970369599</v>
+      </c>
+      <c r="J15">
+        <f>(1000*Export!J15)/[1]Export!J15</f>
+        <v>5.1647194504337364</v>
+      </c>
+      <c r="K15">
+        <f>(1000*Export!K15)/[1]Export!K15</f>
+        <v>4.3136874757658008</v>
+      </c>
+      <c r="L15">
+        <f>(1000*Export!L15)/[1]Export!L15</f>
+        <v>4.917025199754149</v>
+      </c>
+      <c r="M15">
+        <f>(1000*Export!M15)/[1]Export!M15</f>
+        <v>5.3410794602698655</v>
+      </c>
+      <c r="N15">
+        <f>(1000*Export!N15)/[1]Export!N15</f>
+        <v>5.1101884381986586</v>
+      </c>
+      <c r="O15">
+        <f>(1000*Export!O15)/[1]Export!O15</f>
+        <v>3.8657449517918865</v>
+      </c>
+      <c r="P15">
+        <f>(1000*Export!P15)/[1]Export!P15</f>
+        <v>4.3093568055746569</v>
+      </c>
+      <c r="Q15">
+        <f>(1000*Export!Q15)/[1]Export!Q15</f>
+        <v>3.9048473967684023</v>
+      </c>
+      <c r="R15">
+        <f>(1000*Export!R15)/[1]Export!R15</f>
+        <v>4.1490073611420923</v>
+      </c>
+      <c r="S15">
+        <f>(1000*Export!S15)/[1]Export!S15</f>
+        <v>3.7624524349052972</v>
+      </c>
+      <c r="T15">
+        <f>(1000*Export!T15)/[1]Export!T15</f>
+        <v>3.3090391220574684</v>
+      </c>
+      <c r="U15">
+        <f>(1000*Export!U15)/[1]Export!U15</f>
+        <v>3.3649308547745087</v>
+      </c>
+      <c r="V15">
+        <f>(1000*Export!V15)/[1]Export!V15</f>
+        <v>3.1807384144622941</v>
+      </c>
+      <c r="W15">
+        <f>(1000*Export!W15)/[1]Export!W15</f>
+        <v>3.2358628309853597</v>
+      </c>
+      <c r="X15">
+        <f>(1000*Export!X15)/[1]Export!X15</f>
+        <v>3.1122349737405175</v>
+      </c>
+      <c r="Y15">
+        <f>(1000*Export!Y15)/[1]Export!Y15</f>
+        <v>3.954086529233368</v>
+      </c>
+      <c r="Z15">
+        <f>(1000*Export!Z15)/[1]Export!Z15</f>
+        <v>3.4430571320469165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A16" t="str">
+        <f>Export!A16</f>
+        <v>OW</v>
+      </c>
+      <c r="B16">
+        <f>(1000*Export!B16)/[1]Export!B16</f>
+        <v>8.7658056008067646</v>
+      </c>
+      <c r="C16">
+        <f>(1000*Export!C16)/[1]Export!C16</f>
+        <v>8.3752093802345051</v>
+      </c>
+      <c r="D16">
+        <f>(1000*Export!D16)/[1]Export!D16</f>
+        <v>7.3898906296186819</v>
+      </c>
+      <c r="E16">
+        <f>(1000*Export!E16)/[1]Export!E16</f>
+        <v>6.7407673001075654</v>
+      </c>
+      <c r="F16">
+        <f>(1000*Export!F16)/[1]Export!F16</f>
+        <v>7.4079790107261365</v>
+      </c>
+      <c r="G16">
+        <f>(1000*Export!G16)/[1]Export!G16</f>
+        <v>6.2209461307082305</v>
+      </c>
+      <c r="H16">
+        <f>(1000*Export!H16)/[1]Export!H16</f>
+        <v>8.0194083159242542</v>
+      </c>
+      <c r="I16">
+        <f>(1000*Export!I16)/[1]Export!I16</f>
+        <v>5.2113491603937465</v>
+      </c>
+      <c r="J16">
+        <f>(1000*Export!J16)/[1]Export!J16</f>
+        <v>5.7500315935801849</v>
+      </c>
+      <c r="K16">
+        <f>(1000*Export!K16)/[1]Export!K16</f>
+        <v>6.8995256576110391</v>
+      </c>
+      <c r="L16">
+        <f>(1000*Export!L16)/[1]Export!L16</f>
+        <v>4.9246291514023186</v>
+      </c>
+      <c r="M16">
+        <f>(1000*Export!M16)/[1]Export!M16</f>
+        <v>6.1811973862365335</v>
+      </c>
+      <c r="N16">
+        <f>(1000*Export!N16)/[1]Export!N16</f>
+        <v>5.6431438710803423</v>
+      </c>
+      <c r="O16">
+        <f>(1000*Export!O16)/[1]Export!O16</f>
+        <v>5.4006968641114979</v>
+      </c>
+      <c r="P16">
+        <f>(1000*Export!P16)/[1]Export!P16</f>
+        <v>5.7813493669422442</v>
+      </c>
+      <c r="Q16">
+        <f>(1000*Export!Q16)/[1]Export!Q16</f>
+        <v>5.5289139633286322</v>
+      </c>
+      <c r="R16">
+        <f>(1000*Export!R16)/[1]Export!R16</f>
+        <v>4.9631942895382553</v>
+      </c>
+      <c r="S16">
+        <f>(1000*Export!S16)/[1]Export!S16</f>
+        <v>5.8566712810137362</v>
+      </c>
+      <c r="T16">
+        <f>(1000*Export!T16)/[1]Export!T16</f>
+        <v>4.5031214819363425</v>
+      </c>
+      <c r="U16">
+        <f>(1000*Export!U16)/[1]Export!U16</f>
+        <v>4.1272998508204877</v>
+      </c>
+      <c r="V16">
+        <f>(1000*Export!V16)/[1]Export!V16</f>
+        <v>3.8645476063958264</v>
+      </c>
+      <c r="W16">
+        <f>(1000*Export!W16)/[1]Export!W16</f>
+        <v>2.7499881466028162</v>
+      </c>
+      <c r="X16">
+        <f>(1000*Export!X16)/[1]Export!X16</f>
+        <v>2.9365153351356392</v>
+      </c>
+      <c r="Y16">
+        <f>(1000*Export!Y16)/[1]Export!Y16</f>
+        <v>3.0315557392862065</v>
+      </c>
+      <c r="Z16">
+        <f>(1000*Export!Z16)/[1]Export!Z16</f>
+        <v>4.5821613283731057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A17" t="str">
+        <f>Export!A17</f>
+        <v>SH</v>
+      </c>
+      <c r="B17">
+        <f>(1000*Export!B17)/[1]Export!B17</f>
+        <v>5.2509845596049258</v>
+      </c>
+      <c r="C17">
+        <f>(1000*Export!C17)/[1]Export!C17</f>
+        <v>4.7036102544933494</v>
+      </c>
+      <c r="D17">
+        <f>(1000*Export!D17)/[1]Export!D17</f>
+        <v>6.047768158654141</v>
+      </c>
+      <c r="E17">
+        <f>(1000*Export!E17)/[1]Export!E17</f>
+        <v>5.4829571415516769</v>
+      </c>
+      <c r="F17">
+        <f>(1000*Export!F17)/[1]Export!F17</f>
+        <v>5.1098771266540641</v>
+      </c>
+      <c r="G17">
+        <f>(1000*Export!G17)/[1]Export!G17</f>
+        <v>4.8851255329227854</v>
+      </c>
+      <c r="H17">
+        <f>(1000*Export!H17)/[1]Export!H17</f>
+        <v>4.8752176436448051</v>
+      </c>
+      <c r="I17">
+        <f>(1000*Export!I17)/[1]Export!I17</f>
+        <v>4.3532692198258696</v>
+      </c>
+      <c r="J17">
+        <f>(1000*Export!J17)/[1]Export!J17</f>
+        <v>5.6007579135086933</v>
+      </c>
+      <c r="K17">
+        <f>(1000*Export!K17)/[1]Export!K17</f>
+        <v>5.3737043098745225</v>
+      </c>
+      <c r="L17">
+        <f>(1000*Export!L17)/[1]Export!L17</f>
+        <v>5.4111688657870189</v>
+      </c>
+      <c r="M17">
+        <f>(1000*Export!M17)/[1]Export!M17</f>
+        <v>5.3344490350923071</v>
+      </c>
+      <c r="N17">
+        <f>(1000*Export!N17)/[1]Export!N17</f>
+        <v>4.7509618115623953</v>
+      </c>
+      <c r="O17">
+        <f>(1000*Export!O17)/[1]Export!O17</f>
+        <v>5.0307719808983888</v>
+      </c>
+      <c r="P17">
+        <f>(1000*Export!P17)/[1]Export!P17</f>
+        <v>5.3638242758837231</v>
+      </c>
+      <c r="Q17">
+        <f>(1000*Export!Q17)/[1]Export!Q17</f>
+        <v>5.1081962163410939</v>
+      </c>
+      <c r="R17">
+        <f>(1000*Export!R17)/[1]Export!R17</f>
+        <v>4.1550200196419125</v>
+      </c>
+      <c r="S17">
+        <f>(1000*Export!S17)/[1]Export!S17</f>
+        <v>4.2479144275551457</v>
+      </c>
+      <c r="T17">
+        <f>(1000*Export!T17)/[1]Export!T17</f>
+        <v>3.2993475726228572</v>
+      </c>
+      <c r="U17">
+        <f>(1000*Export!U17)/[1]Export!U17</f>
+        <v>3.5475541183000701</v>
+      </c>
+      <c r="V17">
+        <f>(1000*Export!V17)/[1]Export!V17</f>
+        <v>3.9684414418670571</v>
+      </c>
+      <c r="W17">
+        <f>(1000*Export!W17)/[1]Export!W17</f>
+        <v>3.4399404983265156</v>
+      </c>
+      <c r="X17">
+        <f>(1000*Export!X17)/[1]Export!X17</f>
+        <v>3.7227360968368162</v>
+      </c>
+      <c r="Y17">
+        <f>(1000*Export!Y17)/[1]Export!Y17</f>
+        <v>3.566913491060141</v>
+      </c>
+      <c r="Z17">
+        <f>(1000*Export!Z17)/[1]Export!Z17</f>
+        <v>3.7802979764287303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A18" t="str">
+        <f>Export!A18</f>
+        <v>SZ</v>
+      </c>
+      <c r="B18">
+        <f>(1000*Export!B18)/[1]Export!B18</f>
+        <v>7.7452988270340715</v>
+      </c>
+      <c r="C18">
+        <f>(1000*Export!C18)/[1]Export!C18</f>
+        <v>6.7425048225134763</v>
+      </c>
+      <c r="D18">
+        <f>(1000*Export!D18)/[1]Export!D18</f>
+        <v>7.2438470937336357</v>
+      </c>
+      <c r="E18">
+        <f>(1000*Export!E18)/[1]Export!E18</f>
+        <v>7.9124379458158964</v>
+      </c>
+      <c r="F18">
+        <f>(1000*Export!F18)/[1]Export!F18</f>
+        <v>6.5666506773409203</v>
+      </c>
+      <c r="G18">
+        <f>(1000*Export!G18)/[1]Export!G18</f>
+        <v>6.5776714719762106</v>
+      </c>
+      <c r="H18">
+        <f>(1000*Export!H18)/[1]Export!H18</f>
+        <v>6.4027939464493597</v>
+      </c>
+      <c r="I18">
+        <f>(1000*Export!I18)/[1]Export!I18</f>
+        <v>6.3983988840707156</v>
+      </c>
+      <c r="J18">
+        <f>(1000*Export!J18)/[1]Export!J18</f>
+        <v>5.7219345728406683</v>
+      </c>
+      <c r="K18">
+        <f>(1000*Export!K18)/[1]Export!K18</f>
+        <v>5.6170236848807269</v>
+      </c>
+      <c r="L18">
+        <f>(1000*Export!L18)/[1]Export!L18</f>
+        <v>5.6862557033829795</v>
+      </c>
+      <c r="M18">
+        <f>(1000*Export!M18)/[1]Export!M18</f>
+        <v>6.1519449817322158</v>
+      </c>
+      <c r="N18">
+        <f>(1000*Export!N18)/[1]Export!N18</f>
+        <v>5.2832557409635399</v>
+      </c>
+      <c r="O18">
+        <f>(1000*Export!O18)/[1]Export!O18</f>
+        <v>4.7191646949902273</v>
+      </c>
+      <c r="P18">
+        <f>(1000*Export!P18)/[1]Export!P18</f>
+        <v>4.3121471879573487</v>
+      </c>
+      <c r="Q18">
+        <f>(1000*Export!Q18)/[1]Export!Q18</f>
+        <v>4.4857096317457934</v>
+      </c>
+      <c r="R18">
+        <f>(1000*Export!R18)/[1]Export!R18</f>
+        <v>4.4740541531691216</v>
+      </c>
+      <c r="S18">
+        <f>(1000*Export!S18)/[1]Export!S18</f>
+        <v>4.1873225200943347</v>
+      </c>
+      <c r="T18">
+        <f>(1000*Export!T18)/[1]Export!T18</f>
+        <v>4.15096527334918</v>
+      </c>
+      <c r="U18">
+        <f>(1000*Export!U18)/[1]Export!U18</f>
+        <v>3.7023241113857752</v>
+      </c>
+      <c r="V18">
+        <f>(1000*Export!V18)/[1]Export!V18</f>
+        <v>3.4551597051597049</v>
+      </c>
+      <c r="W18">
+        <f>(1000*Export!W18)/[1]Export!W18</f>
+        <v>3.1477049781169826</v>
+      </c>
+      <c r="X18">
+        <f>(1000*Export!X18)/[1]Export!X18</f>
+        <v>2.8689999788265683</v>
+      </c>
+      <c r="Y18">
+        <f>(1000*Export!Y18)/[1]Export!Y18</f>
+        <v>3.0919919483699601</v>
+      </c>
+      <c r="Z18">
+        <f>(1000*Export!Z18)/[1]Export!Z18</f>
+        <v>3.0159326543253755</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A19" t="str">
+        <f>Export!A19</f>
+        <v>SO</v>
+      </c>
+      <c r="B19">
+        <f>(1000*Export!B19)/[1]Export!B19</f>
+        <v>7.1974175628249162</v>
+      </c>
+      <c r="C19">
+        <f>(1000*Export!C19)/[1]Export!C19</f>
+        <v>7.3992953052090273</v>
+      </c>
+      <c r="D19">
+        <f>(1000*Export!D19)/[1]Export!D19</f>
+        <v>7.6224228616431802</v>
+      </c>
+      <c r="E19">
+        <f>(1000*Export!E19)/[1]Export!E19</f>
+        <v>7.2935398771326074</v>
+      </c>
+      <c r="F19">
+        <f>(1000*Export!F19)/[1]Export!F19</f>
+        <v>6.4692351926394478</v>
+      </c>
+      <c r="G19">
+        <f>(1000*Export!G19)/[1]Export!G19</f>
+        <v>7.0381908388138914</v>
+      </c>
+      <c r="H19">
+        <f>(1000*Export!H19)/[1]Export!H19</f>
+        <v>6.5387779846706797</v>
+      </c>
+      <c r="I19">
+        <f>(1000*Export!I19)/[1]Export!I19</f>
+        <v>7.2118023594585239</v>
+      </c>
+      <c r="J19">
+        <f>(1000*Export!J19)/[1]Export!J19</f>
+        <v>7.5138358503171316</v>
+      </c>
+      <c r="K19">
+        <f>(1000*Export!K19)/[1]Export!K19</f>
+        <v>7.122713721698493</v>
+      </c>
+      <c r="L19">
+        <f>(1000*Export!L19)/[1]Export!L19</f>
+        <v>7.2140753225069698</v>
+      </c>
+      <c r="M19">
+        <f>(1000*Export!M19)/[1]Export!M19</f>
+        <v>7.0722997727588925</v>
+      </c>
+      <c r="N19">
+        <f>(1000*Export!N19)/[1]Export!N19</f>
+        <v>7.2266906793241859</v>
+      </c>
+      <c r="O19">
+        <f>(1000*Export!O19)/[1]Export!O19</f>
+        <v>6.5031879106635797</v>
+      </c>
+      <c r="P19">
+        <f>(1000*Export!P19)/[1]Export!P19</f>
+        <v>6.6134686554615545</v>
+      </c>
+      <c r="Q19">
+        <f>(1000*Export!Q19)/[1]Export!Q19</f>
+        <v>7.1412168218621979</v>
+      </c>
+      <c r="R19">
+        <f>(1000*Export!R19)/[1]Export!R19</f>
+        <v>6.2085757791983287</v>
+      </c>
+      <c r="S19">
+        <f>(1000*Export!S19)/[1]Export!S19</f>
+        <v>6.1876100998238401</v>
+      </c>
+      <c r="T19">
+        <f>(1000*Export!T19)/[1]Export!T19</f>
+        <v>6.0487330549676832</v>
+      </c>
+      <c r="U19">
+        <f>(1000*Export!U19)/[1]Export!U19</f>
+        <v>5.52850547939439</v>
+      </c>
+      <c r="V19">
+        <f>(1000*Export!V19)/[1]Export!V19</f>
+        <v>4.6515770147699556</v>
+      </c>
+      <c r="W19">
+        <f>(1000*Export!W19)/[1]Export!W19</f>
+        <v>4.1800946589177599</v>
+      </c>
+      <c r="X19">
+        <f>(1000*Export!X19)/[1]Export!X19</f>
+        <v>3.8974167974673444</v>
+      </c>
+      <c r="Y19">
+        <f>(1000*Export!Y19)/[1]Export!Y19</f>
+        <v>4.0227056468812545</v>
+      </c>
+      <c r="Z19">
+        <f>(1000*Export!Z19)/[1]Export!Z19</f>
+        <v>4.0752896873246884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A20" t="str">
+        <f>Export!A20</f>
+        <v>SG</v>
+      </c>
+      <c r="B20">
+        <f>(1000*Export!B20)/[1]Export!B20</f>
+        <v>7.5774665810586477</v>
+      </c>
+      <c r="C20">
+        <f>(1000*Export!C20)/[1]Export!C20</f>
+        <v>7.5626262106208557</v>
+      </c>
+      <c r="D20">
+        <f>(1000*Export!D20)/[1]Export!D20</f>
+        <v>7.5399353879517532</v>
+      </c>
+      <c r="E20">
+        <f>(1000*Export!E20)/[1]Export!E20</f>
+        <v>6.8794971376280714</v>
+      </c>
+      <c r="F20">
+        <f>(1000*Export!F20)/[1]Export!F20</f>
+        <v>6.2954874330537116</v>
+      </c>
+      <c r="G20">
+        <f>(1000*Export!G20)/[1]Export!G20</f>
+        <v>6.4038264578867903</v>
+      </c>
+      <c r="H20">
+        <f>(1000*Export!H20)/[1]Export!H20</f>
+        <v>6.5855108423147506</v>
+      </c>
+      <c r="I20">
+        <f>(1000*Export!I20)/[1]Export!I20</f>
+        <v>7.206353685823137</v>
+      </c>
+      <c r="J20">
+        <f>(1000*Export!J20)/[1]Export!J20</f>
+        <v>6.897569615271081</v>
+      </c>
+      <c r="K20">
+        <f>(1000*Export!K20)/[1]Export!K20</f>
+        <v>6.8977748804034169</v>
+      </c>
+      <c r="L20">
+        <f>(1000*Export!L20)/[1]Export!L20</f>
+        <v>6.0250803888533682</v>
+      </c>
+      <c r="M20">
+        <f>(1000*Export!M20)/[1]Export!M20</f>
+        <v>6.1622261041801352</v>
+      </c>
+      <c r="N20">
+        <f>(1000*Export!N20)/[1]Export!N20</f>
+        <v>5.7800348151513381</v>
+      </c>
+      <c r="O20">
+        <f>(1000*Export!O20)/[1]Export!O20</f>
+        <v>5.5345530178935674</v>
+      </c>
+      <c r="P20">
+        <f>(1000*Export!P20)/[1]Export!P20</f>
+        <v>5.2330842845713637</v>
+      </c>
+      <c r="Q20">
+        <f>(1000*Export!Q20)/[1]Export!Q20</f>
+        <v>6.0622570448875113</v>
+      </c>
+      <c r="R20">
+        <f>(1000*Export!R20)/[1]Export!R20</f>
+        <v>5.4978356839195826</v>
+      </c>
+      <c r="S20">
+        <f>(1000*Export!S20)/[1]Export!S20</f>
+        <v>5.581344638596403</v>
+      </c>
+      <c r="T20">
+        <f>(1000*Export!T20)/[1]Export!T20</f>
+        <v>4.9212638423244943</v>
+      </c>
+      <c r="U20">
+        <f>(1000*Export!U20)/[1]Export!U20</f>
+        <v>4.9517873104517518</v>
+      </c>
+      <c r="V20">
+        <f>(1000*Export!V20)/[1]Export!V20</f>
+        <v>4.6613581117262051</v>
+      </c>
+      <c r="W20">
+        <f>(1000*Export!W20)/[1]Export!W20</f>
+        <v>3.7000679604319262</v>
+      </c>
+      <c r="X20">
+        <f>(1000*Export!X20)/[1]Export!X20</f>
+        <v>3.6169191439958026</v>
+      </c>
+      <c r="Y20">
+        <f>(1000*Export!Y20)/[1]Export!Y20</f>
+        <v>3.3484399063465986</v>
+      </c>
+      <c r="Z20">
+        <f>(1000*Export!Z20)/[1]Export!Z20</f>
+        <v>3.1742695737564728</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A21" t="str">
+        <f>Export!A21</f>
+        <v>TG</v>
+      </c>
+      <c r="B21">
+        <f>(1000*Export!B21)/[1]Export!B21</f>
+        <v>7.1347121530720061</v>
+      </c>
+      <c r="C21">
+        <f>(1000*Export!C21)/[1]Export!C21</f>
+        <v>7.5818282685076746</v>
+      </c>
+      <c r="D21">
+        <f>(1000*Export!D21)/[1]Export!D21</f>
+        <v>6.5311542997591703</v>
+      </c>
+      <c r="E21">
+        <f>(1000*Export!E21)/[1]Export!E21</f>
+        <v>5.9231156362510164</v>
+      </c>
+      <c r="F21">
+        <f>(1000*Export!F21)/[1]Export!F21</f>
+        <v>5.4161400974905218</v>
+      </c>
+      <c r="G21">
+        <f>(1000*Export!G21)/[1]Export!G21</f>
+        <v>5.872365174810743</v>
+      </c>
+      <c r="H21">
+        <f>(1000*Export!H21)/[1]Export!H21</f>
+        <v>6.0745589703761231</v>
+      </c>
+      <c r="I21">
+        <f>(1000*Export!I21)/[1]Export!I21</f>
+        <v>5.8616541893323282</v>
+      </c>
+      <c r="J21">
+        <f>(1000*Export!J21)/[1]Export!J21</f>
+        <v>5.865333344988243</v>
+      </c>
+      <c r="K21">
+        <f>(1000*Export!K21)/[1]Export!K21</f>
+        <v>5.8829030256144321</v>
+      </c>
+      <c r="L21">
+        <f>(1000*Export!L21)/[1]Export!L21</f>
+        <v>6.1874310549321123</v>
+      </c>
+      <c r="M21">
+        <f>(1000*Export!M21)/[1]Export!M21</f>
+        <v>6.1503509270152952</v>
+      </c>
+      <c r="N21">
+        <f>(1000*Export!N21)/[1]Export!N21</f>
+        <v>5.3350797466635784</v>
+      </c>
+      <c r="O21">
+        <f>(1000*Export!O21)/[1]Export!O21</f>
+        <v>5.4123772521898763</v>
+      </c>
+      <c r="P21">
+        <f>(1000*Export!P21)/[1]Export!P21</f>
+        <v>4.8037691111487471</v>
+      </c>
+      <c r="Q21">
+        <f>(1000*Export!Q21)/[1]Export!Q21</f>
+        <v>5.123176673583715</v>
+      </c>
+      <c r="R21">
+        <f>(1000*Export!R21)/[1]Export!R21</f>
+        <v>4.9765765239853472</v>
+      </c>
+      <c r="S21">
+        <f>(1000*Export!S21)/[1]Export!S21</f>
+        <v>4.3836408304831638</v>
+      </c>
+      <c r="T21">
+        <f>(1000*Export!T21)/[1]Export!T21</f>
+        <v>4.5997644023111013</v>
+      </c>
+      <c r="U21">
+        <f>(1000*Export!U21)/[1]Export!U21</f>
+        <v>4.5288869546295292</v>
+      </c>
+      <c r="V21">
+        <f>(1000*Export!V21)/[1]Export!V21</f>
+        <v>4.0547923564531096</v>
+      </c>
+      <c r="W21">
+        <f>(1000*Export!W21)/[1]Export!W21</f>
+        <v>3.9187423989910366</v>
+      </c>
+      <c r="X21">
+        <f>(1000*Export!X21)/[1]Export!X21</f>
+        <v>3.9616869765809137</v>
+      </c>
+      <c r="Y21">
+        <f>(1000*Export!Y21)/[1]Export!Y21</f>
+        <v>3.6535148278937917</v>
+      </c>
+      <c r="Z21">
+        <f>(1000*Export!Z21)/[1]Export!Z21</f>
+        <v>3.3885113898284791</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A22" t="str">
+        <f>Export!A22</f>
+        <v>TI</v>
+      </c>
+      <c r="B22">
+        <f>(1000*Export!B22)/[1]Export!B22</f>
+        <v>11.261604985374539</v>
+      </c>
+      <c r="C22">
+        <f>(1000*Export!C22)/[1]Export!C22</f>
+        <v>10.761418783453772</v>
+      </c>
+      <c r="D22">
+        <f>(1000*Export!D22)/[1]Export!D22</f>
+        <v>10.75406634319021</v>
+      </c>
+      <c r="E22">
+        <f>(1000*Export!E22)/[1]Export!E22</f>
+        <v>10.193302737510519</v>
+      </c>
+      <c r="F22">
+        <f>(1000*Export!F22)/[1]Export!F22</f>
+        <v>9.6436379022589964</v>
+      </c>
+      <c r="G22">
+        <f>(1000*Export!G22)/[1]Export!G22</f>
+        <v>9.4157048162054426</v>
+      </c>
+      <c r="H22">
+        <f>(1000*Export!H22)/[1]Export!H22</f>
+        <v>8.8250857757369889</v>
+      </c>
+      <c r="I22">
+        <f>(1000*Export!I22)/[1]Export!I22</f>
+        <v>9.002530742388263</v>
+      </c>
+      <c r="J22">
+        <f>(1000*Export!J22)/[1]Export!J22</f>
+        <v>9.1335202383038379</v>
+      </c>
+      <c r="K22">
+        <f>(1000*Export!K22)/[1]Export!K22</f>
+        <v>8.7913151484845056</v>
+      </c>
+      <c r="L22">
+        <f>(1000*Export!L22)/[1]Export!L22</f>
+        <v>8.5694995986369609</v>
+      </c>
+      <c r="M22">
+        <f>(1000*Export!M22)/[1]Export!M22</f>
+        <v>8.0932770076634046</v>
+      </c>
+      <c r="N22">
+        <f>(1000*Export!N22)/[1]Export!N22</f>
+        <v>7.6649400931303298</v>
+      </c>
+      <c r="O22">
+        <f>(1000*Export!O22)/[1]Export!O22</f>
+        <v>7.0381747287639493</v>
+      </c>
+      <c r="P22">
+        <f>(1000*Export!P22)/[1]Export!P22</f>
+        <v>7.709504637469113</v>
+      </c>
+      <c r="Q22">
+        <f>(1000*Export!Q22)/[1]Export!Q22</f>
+        <v>6.8037823393537415</v>
+      </c>
+      <c r="R22">
+        <f>(1000*Export!R22)/[1]Export!R22</f>
+        <v>6.276171535363428</v>
+      </c>
+      <c r="S22">
+        <f>(1000*Export!S22)/[1]Export!S22</f>
+        <v>5.7109487895164008</v>
+      </c>
+      <c r="T22">
+        <f>(1000*Export!T22)/[1]Export!T22</f>
+        <v>5.834825053066095</v>
+      </c>
+      <c r="U22">
+        <f>(1000*Export!U22)/[1]Export!U22</f>
+        <v>5.4194031930278035</v>
+      </c>
+      <c r="V22">
+        <f>(1000*Export!V22)/[1]Export!V22</f>
+        <v>4.9599191296995233</v>
+      </c>
+      <c r="W22">
+        <f>(1000*Export!W22)/[1]Export!W22</f>
+        <v>4.43502273297816</v>
+      </c>
+      <c r="X22">
+        <f>(1000*Export!X22)/[1]Export!X22</f>
+        <v>3.9709558168333796</v>
+      </c>
+      <c r="Y22">
+        <f>(1000*Export!Y22)/[1]Export!Y22</f>
+        <v>4.0676196775601481</v>
+      </c>
+      <c r="Z22">
+        <f>(1000*Export!Z22)/[1]Export!Z22</f>
+        <v>3.2240108654509831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A23" t="str">
+        <f>Export!A23</f>
+        <v>UR</v>
+      </c>
+      <c r="B23">
+        <f>(1000*Export!B23)/[1]Export!B23</f>
+        <v>9.7525473071324598</v>
+      </c>
+      <c r="C23">
+        <f>(1000*Export!C23)/[1]Export!C23</f>
+        <v>10.189437428243398</v>
+      </c>
+      <c r="D23">
+        <f>(1000*Export!D23)/[1]Export!D23</f>
+        <v>11.413766542959177</v>
+      </c>
+      <c r="E23">
+        <f>(1000*Export!E23)/[1]Export!E23</f>
+        <v>12.707182320441989</v>
+      </c>
+      <c r="F23">
+        <f>(1000*Export!F23)/[1]Export!F23</f>
+        <v>12.394534458299111</v>
+      </c>
+      <c r="G23">
+        <f>(1000*Export!G23)/[1]Export!G23</f>
+        <v>10.991207034372502</v>
+      </c>
+      <c r="H23">
+        <f>(1000*Export!H23)/[1]Export!H23</f>
+        <v>10.602345769001392</v>
+      </c>
+      <c r="I23">
+        <f>(1000*Export!I23)/[1]Export!I23</f>
+        <v>9.8435133770822816</v>
+      </c>
+      <c r="J23">
+        <f>(1000*Export!J23)/[1]Export!J23</f>
+        <v>10.031746031746032</v>
+      </c>
+      <c r="K23">
+        <f>(1000*Export!K23)/[1]Export!K23</f>
+        <v>10.000625039064941</v>
+      </c>
+      <c r="L23">
+        <f>(1000*Export!L23)/[1]Export!L23</f>
+        <v>8.8918869197277246</v>
+      </c>
+      <c r="M23">
+        <f>(1000*Export!M23)/[1]Export!M23</f>
+        <v>9.4663852879107626</v>
+      </c>
+      <c r="N23">
+        <f>(1000*Export!N23)/[1]Export!N23</f>
+        <v>6.9519357545247509</v>
+      </c>
+      <c r="O23">
+        <f>(1000*Export!O23)/[1]Export!O23</f>
+        <v>7.0722205573868742</v>
+      </c>
+      <c r="P23">
+        <f>(1000*Export!P23)/[1]Export!P23</f>
+        <v>6.4444169042012645</v>
+      </c>
+      <c r="Q23">
+        <f>(1000*Export!Q23)/[1]Export!Q23</f>
+        <v>7.7761449914278717</v>
+      </c>
+      <c r="R23">
+        <f>(1000*Export!R23)/[1]Export!R23</f>
+        <v>7.0418223011450616</v>
+      </c>
+      <c r="S23">
+        <f>(1000*Export!S23)/[1]Export!S23</f>
+        <v>8.6426914153132248</v>
+      </c>
+      <c r="T23">
+        <f>(1000*Export!T23)/[1]Export!T23</f>
+        <v>6.1585400305101983</v>
+      </c>
+      <c r="U23">
+        <f>(1000*Export!U23)/[1]Export!U23</f>
+        <v>5.8271824185581886</v>
+      </c>
+      <c r="V23">
+        <f>(1000*Export!V23)/[1]Export!V23</f>
+        <v>5.7471264367816088</v>
+      </c>
+      <c r="W23">
+        <f>(1000*Export!W23)/[1]Export!W23</f>
+        <v>6.5579014715291111</v>
+      </c>
+      <c r="X23">
+        <f>(1000*Export!X23)/[1]Export!X23</f>
+        <v>4.9426858765380164</v>
+      </c>
+      <c r="Y23">
+        <f>(1000*Export!Y23)/[1]Export!Y23</f>
+        <v>6.0477618112271267</v>
+      </c>
+      <c r="Z23">
+        <f>(1000*Export!Z23)/[1]Export!Z23</f>
+        <v>5.2139242447477381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A24" t="str">
+        <f>Export!A24</f>
+        <v>VS</v>
+      </c>
+      <c r="B24">
+        <f>(1000*Export!B24)/[1]Export!B24</f>
+        <v>6.8539502675480009</v>
+      </c>
+      <c r="C24">
+        <f>(1000*Export!C24)/[1]Export!C24</f>
+        <v>7.1207092662708984</v>
+      </c>
+      <c r="D24">
+        <f>(1000*Export!D24)/[1]Export!D24</f>
+        <v>6.2847400090218892</v>
+      </c>
+      <c r="E24">
+        <f>(1000*Export!E24)/[1]Export!E24</f>
+        <v>5.940698295245185</v>
+      </c>
+      <c r="F24">
+        <f>(1000*Export!F24)/[1]Export!F24</f>
+        <v>5.1783448366914335</v>
+      </c>
+      <c r="G24">
+        <f>(1000*Export!G24)/[1]Export!G24</f>
+        <v>5.2819692449594307</v>
+      </c>
+      <c r="H24">
+        <f>(1000*Export!H24)/[1]Export!H24</f>
+        <v>5.2641936436091701</v>
+      </c>
+      <c r="I24">
+        <f>(1000*Export!I24)/[1]Export!I24</f>
+        <v>4.8977970188513806</v>
+      </c>
+      <c r="J24">
+        <f>(1000*Export!J24)/[1]Export!J24</f>
+        <v>5.4223878689208371</v>
+      </c>
+      <c r="K24">
+        <f>(1000*Export!K24)/[1]Export!K24</f>
+        <v>4.9744722406097823</v>
+      </c>
+      <c r="L24">
+        <f>(1000*Export!L24)/[1]Export!L24</f>
+        <v>5.2430247335381157</v>
+      </c>
+      <c r="M24">
+        <f>(1000*Export!M24)/[1]Export!M24</f>
+        <v>4.7396316664694416</v>
+      </c>
+      <c r="N24">
+        <f>(1000*Export!N24)/[1]Export!N24</f>
+        <v>4.3952276887101416</v>
+      </c>
+      <c r="O24">
+        <f>(1000*Export!O24)/[1]Export!O24</f>
+        <v>3.7258584173801395</v>
+      </c>
+      <c r="P24">
+        <f>(1000*Export!P24)/[1]Export!P24</f>
+        <v>3.6390912234026969</v>
+      </c>
+      <c r="Q24">
+        <f>(1000*Export!Q24)/[1]Export!Q24</f>
+        <v>3.6607722677823307</v>
+      </c>
+      <c r="R24">
+        <f>(1000*Export!R24)/[1]Export!R24</f>
+        <v>3.3655078158366791</v>
+      </c>
+      <c r="S24">
+        <f>(1000*Export!S24)/[1]Export!S24</f>
+        <v>3.3162279975721458</v>
+      </c>
+      <c r="T24">
+        <f>(1000*Export!T24)/[1]Export!T24</f>
+        <v>3.1800786934727538</v>
+      </c>
+      <c r="U24">
+        <f>(1000*Export!U24)/[1]Export!U24</f>
+        <v>2.9502683960983354</v>
+      </c>
+      <c r="V24">
+        <f>(1000*Export!V24)/[1]Export!V24</f>
+        <v>2.8071133770332604</v>
+      </c>
+      <c r="W24">
+        <f>(1000*Export!W24)/[1]Export!W24</f>
+        <v>2.4729367365180255</v>
+      </c>
+      <c r="X24">
+        <f>(1000*Export!X24)/[1]Export!X24</f>
+        <v>2.5844203340241374</v>
+      </c>
+      <c r="Y24">
+        <f>(1000*Export!Y24)/[1]Export!Y24</f>
+        <v>2.4112032620476604</v>
+      </c>
+      <c r="Z24">
+        <f>(1000*Export!Z24)/[1]Export!Z24</f>
+        <v>2.1955798156461981</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A25" t="str">
+        <f>Export!A25</f>
+        <v>VD</v>
+      </c>
+      <c r="B25">
+        <f>(1000*Export!B25)/[1]Export!B25</f>
+        <v>9.5566754693292086</v>
+      </c>
+      <c r="C25">
+        <f>(1000*Export!C25)/[1]Export!C25</f>
+        <v>9.1837664659324325</v>
+      </c>
+      <c r="D25">
+        <f>(1000*Export!D25)/[1]Export!D25</f>
+        <v>9.1909233607798857</v>
+      </c>
+      <c r="E25">
+        <f>(1000*Export!E25)/[1]Export!E25</f>
+        <v>8.7901247913950016</v>
+      </c>
+      <c r="F25">
+        <f>(1000*Export!F25)/[1]Export!F25</f>
+        <v>7.7980280848521062</v>
+      </c>
+      <c r="G25">
+        <f>(1000*Export!G25)/[1]Export!G25</f>
+        <v>7.5588918840513575</v>
+      </c>
+      <c r="H25">
+        <f>(1000*Export!H25)/[1]Export!H25</f>
+        <v>7.7346090222202353</v>
+      </c>
+      <c r="I25">
+        <f>(1000*Export!I25)/[1]Export!I25</f>
+        <v>7.9642922365948863</v>
+      </c>
+      <c r="J25">
+        <f>(1000*Export!J25)/[1]Export!J25</f>
+        <v>8.2170486369437548</v>
+      </c>
+      <c r="K25">
+        <f>(1000*Export!K25)/[1]Export!K25</f>
+        <v>7.5112535625183119</v>
+      </c>
+      <c r="L25">
+        <f>(1000*Export!L25)/[1]Export!L25</f>
+        <v>7.3896731434577596</v>
+      </c>
+      <c r="M25">
+        <f>(1000*Export!M25)/[1]Export!M25</f>
+        <v>6.9606368939631356</v>
+      </c>
+      <c r="N25">
+        <f>(1000*Export!N25)/[1]Export!N25</f>
+        <v>6.6634760519824763</v>
+      </c>
+      <c r="O25">
+        <f>(1000*Export!O25)/[1]Export!O25</f>
+        <v>5.9632936816205699</v>
+      </c>
+      <c r="P25">
+        <f>(1000*Export!P25)/[1]Export!P25</f>
+        <v>6.0379332302374236</v>
+      </c>
+      <c r="Q25">
+        <f>(1000*Export!Q25)/[1]Export!Q25</f>
+        <v>6.4485116981174508</v>
+      </c>
+      <c r="R25">
+        <f>(1000*Export!R25)/[1]Export!R25</f>
+        <v>5.6575558694026755</v>
+      </c>
+      <c r="S25">
+        <f>(1000*Export!S25)/[1]Export!S25</f>
+        <v>5.6830735583256189</v>
+      </c>
+      <c r="T25">
+        <f>(1000*Export!T25)/[1]Export!T25</f>
+        <v>5.4013229287657936</v>
+      </c>
+      <c r="U25">
+        <f>(1000*Export!U25)/[1]Export!U25</f>
+        <v>4.8002258929831996</v>
+      </c>
+      <c r="V25">
+        <f>(1000*Export!V25)/[1]Export!V25</f>
+        <v>4.5699490754821452</v>
+      </c>
+      <c r="W25">
+        <f>(1000*Export!W25)/[1]Export!W25</f>
+        <v>4.5489355184561191</v>
+      </c>
+      <c r="X25">
+        <f>(1000*Export!X25)/[1]Export!X25</f>
+        <v>4.0472794685461739</v>
+      </c>
+      <c r="Y25">
+        <f>(1000*Export!Y25)/[1]Export!Y25</f>
+        <v>3.4675008482993146</v>
+      </c>
+      <c r="Z25">
+        <f>(1000*Export!Z25)/[1]Export!Z25</f>
+        <v>4.1239827143703245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A26" t="str">
+        <f>Export!A26</f>
+        <v>ZG</v>
+      </c>
+      <c r="B26">
+        <f>(1000*Export!B26)/[1]Export!B26</f>
+        <v>7.2590560862574485</v>
+      </c>
+      <c r="C26">
+        <f>(1000*Export!C26)/[1]Export!C26</f>
+        <v>7.1514256713112481</v>
+      </c>
+      <c r="D26">
+        <f>(1000*Export!D26)/[1]Export!D26</f>
+        <v>5.6009177407382413</v>
+      </c>
+      <c r="E26">
+        <f>(1000*Export!E26)/[1]Export!E26</f>
+        <v>7.124380726906046</v>
+      </c>
+      <c r="F26">
+        <f>(1000*Export!F26)/[1]Export!F26</f>
+        <v>5.998812955740207</v>
+      </c>
+      <c r="G26">
+        <f>(1000*Export!G26)/[1]Export!G26</f>
+        <v>6.2748163844713725</v>
+      </c>
+      <c r="H26">
+        <f>(1000*Export!H26)/[1]Export!H26</f>
+        <v>6.3299903072023422</v>
+      </c>
+      <c r="I26">
+        <f>(1000*Export!I26)/[1]Export!I26</f>
+        <v>5.8171587171834309</v>
+      </c>
+      <c r="J26">
+        <f>(1000*Export!J26)/[1]Export!J26</f>
+        <v>5.6953448339010366</v>
+      </c>
+      <c r="K26">
+        <f>(1000*Export!K26)/[1]Export!K26</f>
+        <v>5.6556087732631095</v>
+      </c>
+      <c r="L26">
+        <f>(1000*Export!L26)/[1]Export!L26</f>
+        <v>5.3802255225522551</v>
+      </c>
+      <c r="M26">
+        <f>(1000*Export!M26)/[1]Export!M26</f>
+        <v>5.0652082456878418</v>
+      </c>
+      <c r="N26">
+        <f>(1000*Export!N26)/[1]Export!N26</f>
+        <v>5.7014427128951759</v>
+      </c>
+      <c r="O26">
+        <f>(1000*Export!O26)/[1]Export!O26</f>
+        <v>5.0638202102691059</v>
+      </c>
+      <c r="P26">
+        <f>(1000*Export!P26)/[1]Export!P26</f>
+        <v>5.4579511690995997</v>
+      </c>
+      <c r="Q26">
+        <f>(1000*Export!Q26)/[1]Export!Q26</f>
+        <v>5.3003533568904597</v>
+      </c>
+      <c r="R26">
+        <f>(1000*Export!R26)/[1]Export!R26</f>
+        <v>5.2337484414205013</v>
+      </c>
+      <c r="S26">
+        <f>(1000*Export!S26)/[1]Export!S26</f>
+        <v>5.3254347058733256</v>
+      </c>
+      <c r="T26">
+        <f>(1000*Export!T26)/[1]Export!T26</f>
+        <v>4.9878290996520462</v>
+      </c>
+      <c r="U26">
+        <f>(1000*Export!U26)/[1]Export!U26</f>
+        <v>4.5534302991632707</v>
+      </c>
+      <c r="V26">
+        <f>(1000*Export!V26)/[1]Export!V26</f>
+        <v>3.9262042470553467</v>
+      </c>
+      <c r="W26">
+        <f>(1000*Export!W26)/[1]Export!W26</f>
+        <v>3.4904493610004121</v>
+      </c>
+      <c r="X26">
+        <f>(1000*Export!X26)/[1]Export!X26</f>
+        <v>3.6899382336426108</v>
+      </c>
+      <c r="Y26">
+        <f>(1000*Export!Y26)/[1]Export!Y26</f>
+        <v>3.469469963745988</v>
+      </c>
+      <c r="Z26">
+        <f>(1000*Export!Z26)/[1]Export!Z26</f>
+        <v>3.399168530523017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A27" t="str">
+        <f>Export!A27</f>
+        <v>ZH</v>
+      </c>
+      <c r="B27">
+        <f>(1000*Export!B27)/[1]Export!B27</f>
+        <v>5.9438040345821328</v>
+      </c>
+      <c r="C27">
+        <f>(1000*Export!C27)/[1]Export!C27</f>
+        <v>5.6811311592770375</v>
+      </c>
+      <c r="D27">
+        <f>(1000*Export!D27)/[1]Export!D27</f>
+        <v>5.9417875398725215</v>
+      </c>
+      <c r="E27">
+        <f>(1000*Export!E27)/[1]Export!E27</f>
+        <v>5.718644898322828</v>
+      </c>
+      <c r="F27">
+        <f>(1000*Export!F27)/[1]Export!F27</f>
+        <v>5.3366353993162097</v>
+      </c>
+      <c r="G27">
+        <f>(1000*Export!G27)/[1]Export!G27</f>
+        <v>5.6082572638864026</v>
+      </c>
+      <c r="H27">
+        <f>(1000*Export!H27)/[1]Export!H27</f>
+        <v>5.4865431766323223</v>
+      </c>
+      <c r="I27">
+        <f>(1000*Export!I27)/[1]Export!I27</f>
+        <v>5.6873991972157212</v>
+      </c>
+      <c r="J27">
+        <f>(1000*Export!J27)/[1]Export!J27</f>
+        <v>5.6994573073915209</v>
+      </c>
+      <c r="K27">
+        <f>(1000*Export!K27)/[1]Export!K27</f>
+        <v>5.6086452317442719</v>
+      </c>
+      <c r="L27">
+        <f>(1000*Export!L27)/[1]Export!L27</f>
+        <v>5.3820859675194921</v>
+      </c>
+      <c r="M27">
+        <f>(1000*Export!M27)/[1]Export!M27</f>
+        <v>5.7523303118748776</v>
+      </c>
+      <c r="N27">
+        <f>(1000*Export!N27)/[1]Export!N27</f>
+        <v>5.4229199926244505</v>
+      </c>
+      <c r="O27">
+        <f>(1000*Export!O27)/[1]Export!O27</f>
+        <v>4.8410233726820069</v>
+      </c>
+      <c r="P27">
+        <f>(1000*Export!P27)/[1]Export!P27</f>
+        <v>4.8851503876392641</v>
+      </c>
+      <c r="Q27">
+        <f>(1000*Export!Q27)/[1]Export!Q27</f>
+        <v>4.8700048003698067</v>
+      </c>
+      <c r="R27">
+        <f>(1000*Export!R27)/[1]Export!R27</f>
+        <v>4.6789265055553804</v>
+      </c>
+      <c r="S27">
+        <f>(1000*Export!S27)/[1]Export!S27</f>
+        <v>4.8951600907084547</v>
+      </c>
+      <c r="T27">
+        <f>(1000*Export!T27)/[1]Export!T27</f>
+        <v>4.5325457400195104</v>
+      </c>
+      <c r="U27">
+        <f>(1000*Export!U27)/[1]Export!U27</f>
+        <v>4.420395458087695</v>
+      </c>
+      <c r="V27">
+        <f>(1000*Export!V27)/[1]Export!V27</f>
+        <v>4.2371415724118844</v>
+      </c>
+      <c r="W27">
+        <f>(1000*Export!W27)/[1]Export!W27</f>
+        <v>4.0418066804577579</v>
+      </c>
+      <c r="X27">
+        <f>(1000*Export!X27)/[1]Export!X27</f>
+        <v>4.2933225012975873</v>
+      </c>
+      <c r="Y27">
+        <f>(1000*Export!Y27)/[1]Export!Y27</f>
+        <v>4.4245036251359338</v>
+      </c>
+      <c r="Z27">
+        <f>(1000*Export!Z27)/[1]Export!Z27</f>
+        <v>4.6586290515386457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>